<commit_message>
sync 30/07/23. add conversation panel. modified case data. bugfixes.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data_telepresence.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data_telepresence.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="43">
   <si>
     <t xml:space="preserve">case_id</t>
   </si>
@@ -147,6 +147,9 @@
   <si>
     <t xml:space="preserve">bedroom_close_bed</t>
   </si>
+  <si>
+    <t xml:space="preserve">decline_instruction_end_call             </t>
+  </si>
 </sst>
 </file>
 
@@ -241,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,6 +365,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,10 +386,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W153"/>
+  <dimension ref="A1:W211"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D156" activeCellId="0" sqref="D156"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H161" activeCellId="0" sqref="H161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5548,264 +5555,368 @@
       <c r="A92" s="18" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C92" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="D92" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E92" s="19" t="s">
+      <c r="B92" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C92" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E92" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F92" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G92" s="18"/>
-      <c r="H92" s="28"/>
-      <c r="I92" s="18"/>
-      <c r="J92" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K92" s="18"/>
-      <c r="L92" s="21"/>
-      <c r="M92" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N92" s="29"/>
-      <c r="O92" s="26"/>
-      <c r="P92" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q92" s="25"/>
-      <c r="R92" s="18"/>
-      <c r="S92" s="19"/>
-      <c r="U92" s="11" t="s">
+      <c r="F92" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H92" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J92" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K92" s="0"/>
+      <c r="L92" s="0"/>
+      <c r="M92" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N92" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="O92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q92" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R92" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="S92" s="0"/>
+      <c r="T92" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="U92" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="V92" s="1" t="n">
-        <v>1</v>
+      <c r="V92" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="18" t="n">
         <v>92</v>
       </c>
-      <c r="B93" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C93" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="D93" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E93" s="19" t="s">
+      <c r="B93" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F93" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G93" s="18"/>
-      <c r="H93" s="28"/>
-      <c r="I93" s="18"/>
-      <c r="J93" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K93" s="18"/>
-      <c r="L93" s="21"/>
-      <c r="M93" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N93" s="29"/>
-      <c r="O93" s="26"/>
-      <c r="P93" s="24" t="n">
+      <c r="F93" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H93" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J93" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K93" s="0"/>
+      <c r="L93" s="0"/>
+      <c r="M93" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N93" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="O93" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P93" s="0" t="n">
         <v>-1</v>
       </c>
-      <c r="Q93" s="25"/>
-      <c r="R93" s="18"/>
-      <c r="S93" s="19"/>
-      <c r="U93" s="11" t="s">
+      <c r="Q93" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R93" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S93" s="0"/>
+      <c r="T93" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U93" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="V93" s="1" t="n">
-        <v>0</v>
+      <c r="V93" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="18" t="n">
         <v>93</v>
       </c>
-      <c r="B94" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C94" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D94" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E94" s="19"/>
-      <c r="F94" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G94" s="18"/>
-      <c r="H94" s="28"/>
-      <c r="I94" s="18"/>
-      <c r="J94" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K94" s="18"/>
-      <c r="L94" s="21"/>
-      <c r="M94" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N94" s="29"/>
-      <c r="O94" s="26"/>
-      <c r="P94" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q94" s="25"/>
-      <c r="R94" s="18"/>
-      <c r="S94" s="19"/>
-      <c r="U94" s="11" t="s">
+      <c r="B94" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C94" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" s="0"/>
+      <c r="F94" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H94" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J94" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K94" s="0"/>
+      <c r="L94" s="0"/>
+      <c r="M94" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N94" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="O94" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P94" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R94" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="S94" s="0"/>
+      <c r="T94" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="U94" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="V94" s="1" t="n">
-        <v>1</v>
+      <c r="V94" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="18" t="n">
         <v>94</v>
       </c>
-      <c r="B95" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C95" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D95" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E95" s="19"/>
-      <c r="F95" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G95" s="18"/>
-      <c r="H95" s="28"/>
-      <c r="I95" s="18"/>
-      <c r="J95" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K95" s="18"/>
-      <c r="M95" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N95" s="29"/>
-      <c r="O95" s="26"/>
-      <c r="P95" s="24" t="n">
+      <c r="B95" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E95" s="0"/>
+      <c r="F95" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H95" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J95" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K95" s="0"/>
+      <c r="L95" s="0"/>
+      <c r="M95" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N95" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="O95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P95" s="0" t="n">
         <v>-1</v>
       </c>
-      <c r="Q95" s="25"/>
-      <c r="R95" s="18"/>
-      <c r="S95" s="19"/>
-      <c r="U95" s="11" t="s">
+      <c r="Q95" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R95" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S95" s="0"/>
+      <c r="T95" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U95" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="V95" s="1" t="n">
-        <v>0</v>
+      <c r="V95" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="18" t="n">
         <v>95</v>
       </c>
-      <c r="B96" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C96" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D96" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E96" s="19" t="s">
+      <c r="B96" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F96" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G96" s="18"/>
-      <c r="H96" s="28"/>
-      <c r="I96" s="18"/>
-      <c r="J96" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K96" s="18"/>
-      <c r="L96" s="21"/>
-      <c r="M96" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N96" s="29"/>
-      <c r="O96" s="18"/>
-      <c r="P96" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q96" s="25"/>
-      <c r="R96" s="18"/>
-      <c r="S96" s="19"/>
-      <c r="U96" s="11" t="s">
+      <c r="F96" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H96" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J96" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K96" s="0"/>
+      <c r="L96" s="0"/>
+      <c r="M96" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N96" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="O96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P96" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R96" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="S96" s="0"/>
+      <c r="T96" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="U96" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="V96" s="1" t="n">
-        <v>1</v>
+      <c r="V96" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="18" t="n">
         <v>96</v>
       </c>
-      <c r="B97" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C97" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D97" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E97" s="19" t="s">
+      <c r="B97" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F97" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G97" s="18"/>
-      <c r="H97" s="28"/>
-      <c r="I97" s="18"/>
-      <c r="J97" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K97" s="18"/>
-      <c r="M97" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N97" s="29"/>
-      <c r="O97" s="26"/>
-      <c r="P97" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q97" s="25"/>
-      <c r="R97" s="18"/>
-      <c r="S97" s="19"/>
-      <c r="U97" s="11" t="s">
+      <c r="F97" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H97" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I97" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J97" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K97" s="0"/>
+      <c r="L97" s="0"/>
+      <c r="M97" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N97" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="O97" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P97" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R97" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S97" s="0"/>
+      <c r="T97" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U97" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="V97" s="1" t="n">
-        <v>0</v>
+      <c r="V97" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5816,12 +5927,14 @@
         <v>23</v>
       </c>
       <c r="C98" s="28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E98" s="19"/>
+      <c r="E98" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="F98" s="28" t="b">
         <v>0</v>
       </c>
@@ -5832,19 +5945,20 @@
         <v>0</v>
       </c>
       <c r="K98" s="18"/>
+      <c r="L98" s="21"/>
       <c r="M98" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N98" s="29"/>
       <c r="O98" s="26"/>
       <c r="P98" s="24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q98" s="25"/>
       <c r="R98" s="18"/>
       <c r="S98" s="19"/>
       <c r="U98" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V98" s="1" t="n">
         <v>1</v>
@@ -5858,12 +5972,14 @@
         <v>23</v>
       </c>
       <c r="C99" s="28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E99" s="19"/>
+      <c r="E99" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="F99" s="28" t="b">
         <v>0</v>
       </c>
@@ -5874,6 +5990,7 @@
         <v>0</v>
       </c>
       <c r="K99" s="18"/>
+      <c r="L99" s="21"/>
       <c r="M99" s="21" t="b">
         <v>0</v>
       </c>
@@ -5905,9 +6022,7 @@
       <c r="D100" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E100" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E100" s="19"/>
       <c r="F100" s="28" t="b">
         <v>0</v>
       </c>
@@ -5931,7 +6046,7 @@
       <c r="R100" s="18"/>
       <c r="S100" s="19"/>
       <c r="U100" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V100" s="1" t="n">
         <v>1</v>
@@ -5950,9 +6065,7 @@
       <c r="D101" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E101" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E101" s="19"/>
       <c r="F101" s="28" t="b">
         <v>0</v>
       </c>
@@ -5963,20 +6076,19 @@
         <v>0</v>
       </c>
       <c r="K101" s="18"/>
-      <c r="L101" s="21"/>
       <c r="M101" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N101" s="29"/>
       <c r="O101" s="26"/>
       <c r="P101" s="24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q101" s="25"/>
       <c r="R101" s="18"/>
       <c r="S101" s="19"/>
       <c r="U101" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V101" s="1" t="n">
         <v>0</v>
@@ -5987,7 +6099,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C102" s="28" t="b">
         <v>1</v>
@@ -5995,7 +6107,9 @@
       <c r="D102" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E102" s="19"/>
+      <c r="E102" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F102" s="28" t="b">
         <v>0</v>
       </c>
@@ -6011,7 +6125,7 @@
         <v>0</v>
       </c>
       <c r="N102" s="29"/>
-      <c r="O102" s="26"/>
+      <c r="O102" s="18"/>
       <c r="P102" s="24" t="n">
         <v>0</v>
       </c>
@@ -6019,7 +6133,7 @@
       <c r="R102" s="18"/>
       <c r="S102" s="19"/>
       <c r="U102" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V102" s="1" t="n">
         <v>1</v>
@@ -6030,7 +6144,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C103" s="28" t="b">
         <v>1</v>
@@ -6038,7 +6152,9 @@
       <c r="D103" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E103" s="19"/>
+      <c r="E103" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F103" s="28" t="b">
         <v>0</v>
       </c>
@@ -6055,13 +6171,13 @@
       <c r="N103" s="29"/>
       <c r="O103" s="26"/>
       <c r="P103" s="24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q103" s="25"/>
       <c r="R103" s="18"/>
       <c r="S103" s="19"/>
       <c r="U103" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V103" s="1" t="n">
         <v>0</v>
@@ -6072,23 +6188,25 @@
         <v>103</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C104" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="D104" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F104" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J104" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="D104" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E104" s="19"/>
+      <c r="F104" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G104" s="18"/>
+      <c r="H104" s="28"/>
+      <c r="I104" s="18"/>
+      <c r="J104" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" s="18"/>
       <c r="M104" s="21" t="b">
         <v>0</v>
       </c>
@@ -6101,7 +6219,7 @@
       <c r="R104" s="18"/>
       <c r="S104" s="19"/>
       <c r="U104" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V104" s="1" t="n">
         <v>1</v>
@@ -6112,7 +6230,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C105" s="28" t="b">
         <v>1</v>
@@ -6120,9 +6238,7 @@
       <c r="D105" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E105" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E105" s="19"/>
       <c r="F105" s="28" t="b">
         <v>0</v>
       </c>
@@ -6133,20 +6249,19 @@
         <v>0</v>
       </c>
       <c r="K105" s="18"/>
-      <c r="L105" s="21"/>
       <c r="M105" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N105" s="29"/>
       <c r="O105" s="26"/>
       <c r="P105" s="24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q105" s="25"/>
       <c r="R105" s="18"/>
       <c r="S105" s="19"/>
       <c r="U105" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V105" s="1" t="n">
         <v>0</v>
@@ -6157,7 +6272,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C106" s="28" t="b">
         <v>1</v>
@@ -6165,28 +6280,20 @@
       <c r="D106" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E106" s="19"/>
+      <c r="E106" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F106" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G106" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H106" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I106" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G106" s="18"/>
+      <c r="H106" s="28"/>
+      <c r="I106" s="18"/>
       <c r="J106" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K106" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L106" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K106" s="18"/>
+      <c r="L106" s="21"/>
       <c r="M106" s="21" t="b">
         <v>0</v>
       </c>
@@ -6195,17 +6302,11 @@
       <c r="P106" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="Q106" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R106" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S106" s="19" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q106" s="25"/>
+      <c r="R106" s="18"/>
+      <c r="S106" s="19"/>
       <c r="U106" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V106" s="1" t="n">
         <v>1</v>
@@ -6216,7 +6317,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C107" s="28" t="b">
         <v>1</v>
@@ -6224,47 +6325,33 @@
       <c r="D107" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E107" s="19"/>
+      <c r="E107" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F107" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G107" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H107" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I107" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G107" s="18"/>
+      <c r="H107" s="28"/>
+      <c r="I107" s="18"/>
       <c r="J107" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K107" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L107" s="21" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K107" s="18"/>
+      <c r="L107" s="21"/>
       <c r="M107" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N107" s="29"/>
-      <c r="O107" s="18"/>
+      <c r="O107" s="26"/>
       <c r="P107" s="24" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q107" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R107" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S107" s="19" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q107" s="25"/>
+      <c r="R107" s="18"/>
+      <c r="S107" s="19"/>
       <c r="U107" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V107" s="1" t="n">
         <v>0</v>
@@ -6283,30 +6370,18 @@
       <c r="D108" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E108" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E108" s="19"/>
       <c r="F108" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H108" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I108" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G108" s="18"/>
+      <c r="H108" s="28"/>
+      <c r="I108" s="18"/>
       <c r="J108" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K108" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L108" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K108" s="18"/>
+      <c r="L108" s="21"/>
       <c r="M108" s="21" t="b">
         <v>0</v>
       </c>
@@ -6315,17 +6390,11 @@
       <c r="P108" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="Q108" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R108" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S108" s="19" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q108" s="25"/>
+      <c r="R108" s="18"/>
+      <c r="S108" s="19"/>
       <c r="U108" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V108" s="1" t="n">
         <v>1</v>
@@ -6344,49 +6413,30 @@
       <c r="D109" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E109" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E109" s="19"/>
       <c r="F109" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G109" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H109" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I109" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G109" s="18"/>
+      <c r="H109" s="28"/>
+      <c r="I109" s="18"/>
       <c r="J109" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K109" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L109" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K109" s="18"/>
       <c r="M109" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N109" s="29"/>
       <c r="O109" s="26"/>
       <c r="P109" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q109" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R109" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S109" s="19" t="n">
-        <v>0</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="Q109" s="25"/>
+      <c r="R109" s="18"/>
+      <c r="S109" s="19"/>
       <c r="U109" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V109" s="1" t="n">
         <v>0</v>
@@ -6402,30 +6452,17 @@
       <c r="C110" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="D110" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E110" s="19"/>
-      <c r="F110" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G110" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H110" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I110" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="J110" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K110" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L110" s="5" t="b">
-        <v>1</v>
+      <c r="D110" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F110" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J110" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="M110" s="21" t="b">
         <v>0</v>
@@ -6435,17 +6472,11 @@
       <c r="P110" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="Q110" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R110" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S110" s="19" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q110" s="25"/>
+      <c r="R110" s="18"/>
+      <c r="S110" s="19"/>
       <c r="U110" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V110" s="1" t="n">
         <v>1</v>
@@ -6464,47 +6495,33 @@
       <c r="D111" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E111" s="19"/>
+      <c r="E111" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F111" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G111" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H111" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I111" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G111" s="18"/>
+      <c r="H111" s="28"/>
+      <c r="I111" s="18"/>
       <c r="J111" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K111" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L111" s="21" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K111" s="18"/>
+      <c r="L111" s="21"/>
       <c r="M111" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N111" s="29"/>
       <c r="O111" s="26"/>
       <c r="P111" s="24" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q111" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R111" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S111" s="19" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q111" s="25"/>
+      <c r="R111" s="18"/>
+      <c r="S111" s="19"/>
       <c r="U111" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V111" s="1" t="n">
         <v>0</v>
@@ -6523,9 +6540,7 @@
       <c r="D112" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E112" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="E112" s="19"/>
       <c r="F112" s="28" t="b">
         <v>1</v>
       </c>
@@ -6565,7 +6580,7 @@
         <v>0</v>
       </c>
       <c r="U112" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="V112" s="1" t="n">
         <v>1</v>
@@ -6584,9 +6599,7 @@
       <c r="D113" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E113" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="E113" s="19"/>
       <c r="F113" s="28" t="b">
         <v>1</v>
       </c>
@@ -6614,7 +6627,7 @@
       <c r="N113" s="29"/>
       <c r="O113" s="18"/>
       <c r="P113" s="24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q113" s="25" t="n">
         <v>-0.5</v>
@@ -6626,7 +6639,7 @@
         <v>0</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V113" s="1" t="n">
         <v>0</v>
@@ -6645,7 +6658,9 @@
       <c r="D114" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E114" s="19"/>
+      <c r="E114" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F114" s="28" t="b">
         <v>1</v>
       </c>
@@ -6685,7 +6700,7 @@
         <v>0</v>
       </c>
       <c r="U114" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V114" s="1" t="n">
         <v>1</v>
@@ -6704,7 +6719,9 @@
       <c r="D115" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E115" s="19"/>
+      <c r="E115" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F115" s="28" t="b">
         <v>1</v>
       </c>
@@ -6732,7 +6749,7 @@
       <c r="N115" s="29"/>
       <c r="O115" s="26"/>
       <c r="P115" s="24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q115" s="25" t="n">
         <v>-0.5</v>
@@ -6744,7 +6761,7 @@
         <v>0</v>
       </c>
       <c r="U115" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V115" s="1" t="n">
         <v>0</v>
@@ -6763,9 +6780,7 @@
       <c r="D116" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E116" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="E116" s="19"/>
       <c r="F116" s="28" t="b">
         <v>1</v>
       </c>
@@ -6805,7 +6820,7 @@
         <v>0</v>
       </c>
       <c r="U116" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="V116" s="1" t="n">
         <v>1</v>
@@ -6824,9 +6839,7 @@
       <c r="D117" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E117" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="E117" s="19"/>
       <c r="F117" s="28" t="b">
         <v>1</v>
       </c>
@@ -6854,7 +6867,7 @@
       <c r="N117" s="29"/>
       <c r="O117" s="26"/>
       <c r="P117" s="24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q117" s="25" t="n">
         <v>-0.5</v>
@@ -6866,7 +6879,7 @@
         <v>0</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V117" s="1" t="n">
         <v>0</v>
@@ -6885,7 +6898,9 @@
       <c r="D118" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E118" s="19"/>
+      <c r="E118" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F118" s="28" t="b">
         <v>1</v>
       </c>
@@ -6904,7 +6919,7 @@
       <c r="K118" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L118" s="21" t="b">
+      <c r="L118" s="5" t="b">
         <v>1</v>
       </c>
       <c r="M118" s="21" t="b">
@@ -6925,7 +6940,7 @@
         <v>0</v>
       </c>
       <c r="U118" s="11" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="V118" s="1" t="n">
         <v>1</v>
@@ -6944,7 +6959,9 @@
       <c r="D119" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E119" s="19"/>
+      <c r="E119" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F119" s="28" t="b">
         <v>1</v>
       </c>
@@ -6970,9 +6987,9 @@
         <v>0</v>
       </c>
       <c r="N119" s="29"/>
-      <c r="O119" s="26"/>
+      <c r="O119" s="18"/>
       <c r="P119" s="24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q119" s="25" t="n">
         <v>-0.5</v>
@@ -6984,7 +7001,7 @@
         <v>0</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V119" s="1" t="n">
         <v>0</v>
@@ -7081,14 +7098,14 @@
       <c r="K121" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L121" s="21" t="b">
+      <c r="L121" s="5" t="b">
         <v>1</v>
       </c>
       <c r="M121" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N121" s="29"/>
-      <c r="O121" s="18"/>
+      <c r="O121" s="26"/>
       <c r="P121" s="24" t="n">
         <v>-1</v>
       </c>
@@ -7113,40 +7130,57 @@
         <v>121</v>
       </c>
       <c r="B122" s="18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C122" s="28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D122" s="19" t="s">
         <v>24</v>
       </c>
       <c r="E122" s="19" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F122" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G122" s="18"/>
-      <c r="H122" s="28"/>
-      <c r="I122" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G122" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H122" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I122" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="J122" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K122" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="K122" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L122" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="M122" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N122" s="29"/>
       <c r="O122" s="26"/>
       <c r="P122" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q122" s="25"/>
-      <c r="R122" s="18"/>
-      <c r="S122" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q122" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R122" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S122" s="19" t="n">
+        <v>0</v>
+      </c>
       <c r="U122" s="11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="V122" s="1" t="n">
         <v>1</v>
@@ -7157,40 +7191,57 @@
         <v>122</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C123" s="28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D123" s="19" t="s">
         <v>24</v>
       </c>
       <c r="E123" s="19" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F123" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G123" s="18"/>
-      <c r="H123" s="28"/>
-      <c r="I123" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G123" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H123" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I123" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="J123" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K123" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="K123" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L123" s="21" t="b">
+        <v>1</v>
+      </c>
       <c r="M123" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N123" s="29"/>
       <c r="O123" s="26"/>
       <c r="P123" s="24" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q123" s="25"/>
-      <c r="R123" s="18"/>
-      <c r="S123" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q123" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R123" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S123" s="19" t="n">
+        <v>0</v>
+      </c>
       <c r="U123" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V123" s="1" t="n">
         <v>0</v>
@@ -7201,7 +7252,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C124" s="28" t="b">
         <v>1</v>
@@ -7211,15 +7262,26 @@
       </c>
       <c r="E124" s="19"/>
       <c r="F124" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G124" s="18"/>
-      <c r="H124" s="28"/>
-      <c r="I124" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G124" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H124" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I124" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="J124" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K124" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="K124" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L124" s="21" t="b">
+        <v>1</v>
+      </c>
       <c r="M124" s="21" t="b">
         <v>0</v>
       </c>
@@ -7228,9 +7290,15 @@
       <c r="P124" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="Q124" s="25"/>
-      <c r="R124" s="18"/>
-      <c r="S124" s="19"/>
+      <c r="Q124" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R124" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S124" s="19" t="n">
+        <v>0</v>
+      </c>
       <c r="U124" s="11" t="s">
         <v>28</v>
       </c>
@@ -7243,7 +7311,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C125" s="28" t="b">
         <v>1</v>
@@ -7253,16 +7321,26 @@
       </c>
       <c r="E125" s="19"/>
       <c r="F125" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G125" s="18"/>
-      <c r="H125" s="28"/>
-      <c r="I125" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G125" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H125" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I125" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="J125" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K125" s="18"/>
-      <c r="L125" s="21"/>
+        <v>1</v>
+      </c>
+      <c r="K125" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L125" s="21" t="b">
+        <v>1</v>
+      </c>
       <c r="M125" s="21" t="b">
         <v>0</v>
       </c>
@@ -7271,9 +7349,15 @@
       <c r="P125" s="24" t="n">
         <v>-1</v>
       </c>
-      <c r="Q125" s="25"/>
-      <c r="R125" s="18"/>
-      <c r="S125" s="19"/>
+      <c r="Q125" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R125" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S125" s="19" t="n">
+        <v>0</v>
+      </c>
       <c r="U125" s="11" t="s">
         <v>27</v>
       </c>
@@ -7286,7 +7370,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C126" s="28" t="b">
         <v>1</v>
@@ -7294,20 +7378,28 @@
       <c r="D126" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E126" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E126" s="19"/>
       <c r="F126" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G126" s="18"/>
-      <c r="H126" s="28"/>
-      <c r="I126" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G126" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H126" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I126" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="J126" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K126" s="18"/>
-      <c r="L126" s="21"/>
+        <v>1</v>
+      </c>
+      <c r="K126" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L126" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="M126" s="21" t="b">
         <v>0</v>
       </c>
@@ -7316,11 +7408,17 @@
       <c r="P126" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="Q126" s="25"/>
-      <c r="R126" s="18"/>
-      <c r="S126" s="19"/>
+      <c r="Q126" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R126" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S126" s="19" t="n">
+        <v>0</v>
+      </c>
       <c r="U126" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V126" s="1" t="n">
         <v>1</v>
@@ -7331,7 +7429,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C127" s="28" t="b">
         <v>1</v>
@@ -7339,33 +7437,47 @@
       <c r="D127" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E127" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E127" s="19"/>
       <c r="F127" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G127" s="18"/>
-      <c r="H127" s="28"/>
-      <c r="I127" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G127" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H127" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I127" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="J127" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K127" s="18"/>
-      <c r="L127" s="21"/>
+        <v>1</v>
+      </c>
+      <c r="K127" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L127" s="21" t="b">
+        <v>1</v>
+      </c>
       <c r="M127" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N127" s="29"/>
-      <c r="O127" s="26"/>
+      <c r="O127" s="18"/>
       <c r="P127" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q127" s="25"/>
-      <c r="R127" s="18"/>
-      <c r="S127" s="19"/>
+        <v>-1</v>
+      </c>
+      <c r="Q127" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R127" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S127" s="19" t="n">
+        <v>0</v>
+      </c>
       <c r="U127" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V127" s="1" t="n">
         <v>0</v>
@@ -7379,12 +7491,14 @@
         <v>23</v>
       </c>
       <c r="C128" s="28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D128" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E128" s="19"/>
+      <c r="E128" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="F128" s="28" t="b">
         <v>0</v>
       </c>
@@ -7401,13 +7515,13 @@
       <c r="N128" s="29"/>
       <c r="O128" s="26"/>
       <c r="P128" s="24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q128" s="25"/>
       <c r="R128" s="18"/>
       <c r="S128" s="19"/>
       <c r="U128" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V128" s="1" t="n">
         <v>1</v>
@@ -7421,17 +7535,24 @@
         <v>23</v>
       </c>
       <c r="C129" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D129" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F129" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J129" s="3" t="b">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D129" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E129" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F129" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G129" s="18"/>
+      <c r="H129" s="28"/>
+      <c r="I129" s="18"/>
+      <c r="J129" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K129" s="18"/>
       <c r="M129" s="21" t="b">
         <v>0</v>
       </c>
@@ -7463,9 +7584,7 @@
       <c r="D130" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E130" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E130" s="19"/>
       <c r="F130" s="28" t="b">
         <v>0</v>
       </c>
@@ -7476,7 +7595,6 @@
         <v>0</v>
       </c>
       <c r="K130" s="18"/>
-      <c r="L130" s="21"/>
       <c r="M130" s="21" t="b">
         <v>0</v>
       </c>
@@ -7489,7 +7607,7 @@
       <c r="R130" s="18"/>
       <c r="S130" s="19"/>
       <c r="U130" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V130" s="1" t="n">
         <v>1</v>
@@ -7508,9 +7626,7 @@
       <c r="D131" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E131" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E131" s="19"/>
       <c r="F131" s="28" t="b">
         <v>0</v>
       </c>
@@ -7521,19 +7637,20 @@
         <v>0</v>
       </c>
       <c r="K131" s="18"/>
+      <c r="L131" s="21"/>
       <c r="M131" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N131" s="29"/>
       <c r="O131" s="26"/>
       <c r="P131" s="24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q131" s="25"/>
       <c r="R131" s="18"/>
       <c r="S131" s="19"/>
       <c r="U131" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V131" s="1" t="n">
         <v>0</v>
@@ -7544,7 +7661,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C132" s="28" t="b">
         <v>1</v>
@@ -7552,7 +7669,9 @@
       <c r="D132" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E132" s="19"/>
+      <c r="E132" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F132" s="28" t="b">
         <v>0</v>
       </c>
@@ -7568,7 +7687,7 @@
         <v>0</v>
       </c>
       <c r="N132" s="29"/>
-      <c r="O132" s="18"/>
+      <c r="O132" s="26"/>
       <c r="P132" s="24" t="n">
         <v>0</v>
       </c>
@@ -7576,7 +7695,7 @@
       <c r="R132" s="18"/>
       <c r="S132" s="19"/>
       <c r="U132" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V132" s="1" t="n">
         <v>1</v>
@@ -7587,7 +7706,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C133" s="28" t="b">
         <v>1</v>
@@ -7595,7 +7714,9 @@
       <c r="D133" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E133" s="19"/>
+      <c r="E133" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F133" s="28" t="b">
         <v>0</v>
       </c>
@@ -7606,19 +7727,20 @@
         <v>0</v>
       </c>
       <c r="K133" s="18"/>
+      <c r="L133" s="21"/>
       <c r="M133" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N133" s="29"/>
       <c r="O133" s="26"/>
       <c r="P133" s="24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q133" s="25"/>
       <c r="R133" s="18"/>
       <c r="S133" s="19"/>
       <c r="U133" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V133" s="1" t="n">
         <v>0</v>
@@ -7629,7 +7751,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C134" s="28" t="b">
         <v>1</v>
@@ -7637,9 +7759,7 @@
       <c r="D134" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E134" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E134" s="19"/>
       <c r="F134" s="28" t="b">
         <v>0</v>
       </c>
@@ -7662,7 +7782,7 @@
       <c r="R134" s="18"/>
       <c r="S134" s="19"/>
       <c r="U134" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V134" s="1" t="n">
         <v>1</v>
@@ -7673,40 +7793,33 @@
         <v>134</v>
       </c>
       <c r="B135" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C135" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="D135" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E135" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F135" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G135" s="18"/>
-      <c r="H135" s="28"/>
-      <c r="I135" s="18"/>
-      <c r="J135" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K135" s="18"/>
+      <c r="D135" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F135" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J135" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="M135" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N135" s="29"/>
       <c r="O135" s="26"/>
       <c r="P135" s="24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q135" s="25"/>
       <c r="R135" s="18"/>
       <c r="S135" s="19"/>
       <c r="U135" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V135" s="1" t="n">
         <v>0</v>
@@ -7717,7 +7830,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C136" s="28" t="b">
         <v>1</v>
@@ -7725,28 +7838,20 @@
       <c r="D136" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E136" s="19"/>
+      <c r="E136" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F136" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G136" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H136" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I136" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G136" s="18"/>
+      <c r="H136" s="28"/>
+      <c r="I136" s="18"/>
       <c r="J136" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K136" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L136" s="21" t="b">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K136" s="18"/>
+      <c r="L136" s="21"/>
       <c r="M136" s="21" t="b">
         <v>0</v>
       </c>
@@ -7755,20 +7860,14 @@
       <c r="P136" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="Q136" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R136" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S136" s="19" t="n">
-        <v>-0.8</v>
-      </c>
+      <c r="Q136" s="25"/>
+      <c r="R136" s="18"/>
+      <c r="S136" s="19"/>
       <c r="U136" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V136" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7776,7 +7875,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C137" s="28" t="b">
         <v>1</v>
@@ -7784,50 +7883,35 @@
       <c r="D137" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E137" s="19"/>
+      <c r="E137" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F137" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G137" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H137" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I137" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G137" s="18"/>
+      <c r="H137" s="28"/>
+      <c r="I137" s="18"/>
       <c r="J137" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K137" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L137" s="5" t="b">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K137" s="18"/>
       <c r="M137" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N137" s="29"/>
       <c r="O137" s="26"/>
       <c r="P137" s="24" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q137" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R137" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S137" s="19" t="n">
-        <v>0.8</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q137" s="25"/>
+      <c r="R137" s="18"/>
+      <c r="S137" s="19"/>
       <c r="U137" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V137" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7843,30 +7927,18 @@
       <c r="D138" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E138" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E138" s="19"/>
       <c r="F138" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G138" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H138" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I138" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G138" s="18"/>
+      <c r="H138" s="28"/>
+      <c r="I138" s="18"/>
       <c r="J138" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K138" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L138" s="21" t="b">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K138" s="18"/>
+      <c r="L138" s="21"/>
       <c r="M138" s="21" t="b">
         <v>0</v>
       </c>
@@ -7875,20 +7947,14 @@
       <c r="P138" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="Q138" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R138" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S138" s="19" t="n">
-        <v>-0.8</v>
-      </c>
+      <c r="Q138" s="25"/>
+      <c r="R138" s="18"/>
+      <c r="S138" s="19"/>
       <c r="U138" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V138" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7904,52 +7970,33 @@
       <c r="D139" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E139" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E139" s="19"/>
       <c r="F139" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G139" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H139" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I139" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G139" s="18"/>
+      <c r="H139" s="28"/>
+      <c r="I139" s="18"/>
       <c r="J139" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K139" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L139" s="5" t="b">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K139" s="18"/>
       <c r="M139" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N139" s="29"/>
       <c r="O139" s="26"/>
       <c r="P139" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q139" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R139" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S139" s="19" t="n">
-        <v>0.8</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="Q139" s="25"/>
+      <c r="R139" s="18"/>
+      <c r="S139" s="19"/>
       <c r="U139" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V139" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7965,28 +8012,19 @@
       <c r="D140" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E140" s="19"/>
+      <c r="E140" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F140" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G140" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H140" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I140" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G140" s="18"/>
+      <c r="H140" s="28"/>
+      <c r="I140" s="18"/>
       <c r="J140" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K140" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L140" s="5" t="b">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K140" s="18"/>
       <c r="M140" s="21" t="b">
         <v>0</v>
       </c>
@@ -7995,20 +8033,14 @@
       <c r="P140" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="Q140" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R140" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S140" s="19" t="n">
-        <v>-0.8</v>
-      </c>
+      <c r="Q140" s="25"/>
+      <c r="R140" s="18"/>
+      <c r="S140" s="19"/>
       <c r="U140" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V140" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8024,50 +8056,35 @@
       <c r="D141" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E141" s="19"/>
+      <c r="E141" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F141" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G141" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H141" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I141" s="18" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G141" s="18"/>
+      <c r="H141" s="28"/>
+      <c r="I141" s="18"/>
       <c r="J141" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K141" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L141" s="5" t="b">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K141" s="18"/>
       <c r="M141" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N141" s="29"/>
       <c r="O141" s="26"/>
       <c r="P141" s="24" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q141" s="25" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="R141" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S141" s="19" t="n">
-        <v>0.8</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q141" s="25"/>
+      <c r="R141" s="18"/>
+      <c r="S141" s="19"/>
       <c r="U141" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V141" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8083,9 +8100,7 @@
       <c r="D142" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E142" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="E142" s="19"/>
       <c r="F142" s="28" t="b">
         <v>1</v>
       </c>
@@ -8122,10 +8137,10 @@
         <v>0</v>
       </c>
       <c r="S142" s="19" t="n">
-        <v>-0.8</v>
+        <v>-0.2</v>
       </c>
       <c r="U142" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="V142" s="1" t="n">
         <v>0</v>
@@ -8144,9 +8159,7 @@
       <c r="D143" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E143" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="E143" s="19"/>
       <c r="F143" s="28" t="b">
         <v>1</v>
       </c>
@@ -8165,7 +8178,7 @@
       <c r="K143" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L143" s="21" t="b">
+      <c r="L143" s="5" t="b">
         <v>0</v>
       </c>
       <c r="M143" s="21" t="b">
@@ -8174,7 +8187,7 @@
       <c r="N143" s="29"/>
       <c r="O143" s="26"/>
       <c r="P143" s="24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q143" s="25" t="n">
         <v>-0.5</v>
@@ -8183,10 +8196,10 @@
         <v>0</v>
       </c>
       <c r="S143" s="19" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="U143" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V143" s="1" t="n">
         <v>1</v>
@@ -8205,7 +8218,9 @@
       <c r="D144" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E144" s="19"/>
+      <c r="E144" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F144" s="28" t="b">
         <v>1</v>
       </c>
@@ -8231,7 +8246,7 @@
         <v>0</v>
       </c>
       <c r="N144" s="29"/>
-      <c r="O144" s="26"/>
+      <c r="O144" s="18"/>
       <c r="P144" s="24" t="n">
         <v>0</v>
       </c>
@@ -8242,10 +8257,10 @@
         <v>0</v>
       </c>
       <c r="S144" s="19" t="n">
-        <v>-0.8</v>
+        <v>-0.2</v>
       </c>
       <c r="U144" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V144" s="1" t="n">
         <v>0</v>
@@ -8264,7 +8279,9 @@
       <c r="D145" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E145" s="19"/>
+      <c r="E145" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="F145" s="28" t="b">
         <v>1</v>
       </c>
@@ -8292,7 +8309,7 @@
       <c r="N145" s="29"/>
       <c r="O145" s="26"/>
       <c r="P145" s="24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q145" s="25" t="n">
         <v>-0.5</v>
@@ -8301,10 +8318,10 @@
         <v>0</v>
       </c>
       <c r="S145" s="19" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="U145" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V145" s="1" t="n">
         <v>1</v>
@@ -8323,9 +8340,7 @@
       <c r="D146" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E146" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="E146" s="19"/>
       <c r="F146" s="28" t="b">
         <v>1</v>
       </c>
@@ -8344,14 +8359,14 @@
       <c r="K146" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L146" s="21" t="b">
+      <c r="L146" s="5" t="b">
         <v>0</v>
       </c>
       <c r="M146" s="21" t="b">
         <v>0</v>
       </c>
       <c r="N146" s="29"/>
-      <c r="O146" s="18"/>
+      <c r="O146" s="26"/>
       <c r="P146" s="24" t="n">
         <v>0</v>
       </c>
@@ -8362,10 +8377,10 @@
         <v>0</v>
       </c>
       <c r="S146" s="19" t="n">
-        <v>-0.8</v>
+        <v>-0.2</v>
       </c>
       <c r="U146" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="V146" s="1" t="n">
         <v>0</v>
@@ -8384,9 +8399,7 @@
       <c r="D147" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E147" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="E147" s="19"/>
       <c r="F147" s="28" t="b">
         <v>1</v>
       </c>
@@ -8414,7 +8427,7 @@
       <c r="N147" s="29"/>
       <c r="O147" s="26"/>
       <c r="P147" s="24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q147" s="25" t="n">
         <v>-0.5</v>
@@ -8423,10 +8436,10 @@
         <v>0</v>
       </c>
       <c r="S147" s="19" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="U147" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V147" s="1" t="n">
         <v>1</v>
@@ -8445,7 +8458,9 @@
       <c r="D148" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E148" s="19"/>
+      <c r="E148" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F148" s="28" t="b">
         <v>1</v>
       </c>
@@ -8464,7 +8479,7 @@
       <c r="K148" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L148" s="5" t="b">
+      <c r="L148" s="21" t="b">
         <v>0</v>
       </c>
       <c r="M148" s="21" t="b">
@@ -8482,10 +8497,10 @@
         <v>0</v>
       </c>
       <c r="S148" s="19" t="n">
-        <v>-0.8</v>
+        <v>-0.2</v>
       </c>
       <c r="U148" s="11" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="V148" s="1" t="n">
         <v>0</v>
@@ -8504,7 +8519,9 @@
       <c r="D149" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E149" s="19"/>
+      <c r="E149" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F149" s="28" t="b">
         <v>1</v>
       </c>
@@ -8523,7 +8540,7 @@
       <c r="K149" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L149" s="5" t="b">
+      <c r="L149" s="21" t="b">
         <v>0</v>
       </c>
       <c r="M149" s="21" t="b">
@@ -8532,7 +8549,7 @@
       <c r="N149" s="29"/>
       <c r="O149" s="26"/>
       <c r="P149" s="24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q149" s="25" t="n">
         <v>-0.5</v>
@@ -8541,10 +8558,10 @@
         <v>0</v>
       </c>
       <c r="S149" s="19" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="U149" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="V149" s="1" t="n">
         <v>1</v>
@@ -8600,7 +8617,7 @@
         <v>0</v>
       </c>
       <c r="S150" s="19" t="n">
-        <v>-0.8</v>
+        <v>-0.2</v>
       </c>
       <c r="U150" s="11" t="s">
         <v>28</v>
@@ -8641,7 +8658,7 @@
       <c r="K151" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L151" s="21" t="b">
+      <c r="L151" s="5" t="b">
         <v>0</v>
       </c>
       <c r="M151" s="21" t="b">
@@ -8659,7 +8676,7 @@
         <v>0</v>
       </c>
       <c r="S151" s="19" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="U151" s="11" t="s">
         <v>27</v>
@@ -8669,43 +8686,1882 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="18"/>
-      <c r="C152" s="28"/>
-      <c r="D152" s="19"/>
-      <c r="E152" s="19"/>
-      <c r="F152" s="28"/>
-      <c r="G152" s="18"/>
-      <c r="H152" s="28"/>
-      <c r="I152" s="18"/>
-      <c r="J152" s="28"/>
-      <c r="K152" s="18"/>
-      <c r="L152" s="21"/>
-      <c r="M152" s="21"/>
+      <c r="A152" s="18" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C152" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D152" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E152" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F152" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G152" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H152" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I152" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J152" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K152" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L152" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M152" s="21" t="b">
+        <v>0</v>
+      </c>
       <c r="N152" s="29"/>
-      <c r="O152" s="26"/>
-      <c r="P152" s="24"/>
-      <c r="Q152" s="25"/>
-      <c r="R152" s="18"/>
-      <c r="S152" s="19"/>
+      <c r="O152" s="18"/>
+      <c r="P152" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R152" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S152" s="19" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="U152" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="V152" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="18"/>
-      <c r="C153" s="28"/>
-      <c r="D153" s="19"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="28"/>
-      <c r="G153" s="18"/>
-      <c r="H153" s="28"/>
-      <c r="I153" s="18"/>
-      <c r="J153" s="28"/>
-      <c r="K153" s="18"/>
-      <c r="M153" s="21"/>
+      <c r="A153" s="18" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C153" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D153" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E153" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F153" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G153" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H153" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I153" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J153" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K153" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L153" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M153" s="21" t="b">
+        <v>0</v>
+      </c>
       <c r="N153" s="29"/>
       <c r="O153" s="26"/>
-      <c r="P153" s="24"/>
-      <c r="Q153" s="25"/>
-      <c r="R153" s="18"/>
-      <c r="S153" s="19"/>
+      <c r="P153" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R153" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S153" s="19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U153" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V153" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="18" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C154" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D154" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E154" s="19"/>
+      <c r="F154" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G154" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H154" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I154" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J154" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K154" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L154" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M154" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N154" s="29"/>
+      <c r="O154" s="26"/>
+      <c r="P154" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q154" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R154" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S154" s="19" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="U154" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V154" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="18" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C155" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D155" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E155" s="19"/>
+      <c r="F155" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G155" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H155" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I155" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J155" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K155" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L155" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M155" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N155" s="29"/>
+      <c r="O155" s="26"/>
+      <c r="P155" s="24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q155" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R155" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S155" s="19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U155" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V155" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="18" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C156" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D156" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E156" s="19"/>
+      <c r="F156" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G156" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H156" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I156" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J156" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K156" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L156" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M156" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N156" s="29"/>
+      <c r="O156" s="26"/>
+      <c r="P156" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q156" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R156" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S156" s="19" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="U156" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V156" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="18" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C157" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D157" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E157" s="19"/>
+      <c r="F157" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G157" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H157" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I157" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J157" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K157" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L157" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M157" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N157" s="29"/>
+      <c r="O157" s="26"/>
+      <c r="P157" s="24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q157" s="25" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R157" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S157" s="19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U157" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V157" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="18" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C158" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D158" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E158" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F158" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G158" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H158" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I158" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J158" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K158" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L158" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M158" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N158" s="0"/>
+      <c r="O158" s="0"/>
+      <c r="P158" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q158" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R158" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S158" s="0" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="T158" s="0"/>
+      <c r="U158" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="V158" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="18" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C159" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D159" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E159" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F159" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G159" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H159" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I159" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J159" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K159" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L159" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M159" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N159" s="0"/>
+      <c r="O159" s="0"/>
+      <c r="P159" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q159" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R159" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S159" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T159" s="0"/>
+      <c r="U159" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="V159" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="18" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C160" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D160" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E160" s="0"/>
+      <c r="F160" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G160" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H160" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I160" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J160" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K160" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L160" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M160" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N160" s="0"/>
+      <c r="O160" s="0"/>
+      <c r="P160" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q160" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R160" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S160" s="0" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="T160" s="0"/>
+      <c r="U160" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="V160" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="18" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C161" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D161" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E161" s="0"/>
+      <c r="F161" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G161" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H161" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I161" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J161" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K161" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L161" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M161" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N161" s="0"/>
+      <c r="O161" s="0"/>
+      <c r="P161" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q161" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S161" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T161" s="0"/>
+      <c r="U161" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="V161" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="18" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C162" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D162" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E162" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F162" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G162" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H162" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I162" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J162" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K162" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L162" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M162" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N162" s="0"/>
+      <c r="O162" s="0"/>
+      <c r="P162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q162" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S162" s="0" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="T162" s="0"/>
+      <c r="U162" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="V162" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="18" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C163" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D163" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E163" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F163" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G163" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H163" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I163" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J163" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K163" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L163" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M163" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N163" s="0"/>
+      <c r="O163" s="0"/>
+      <c r="P163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q163" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="R163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S163" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T163" s="0"/>
+      <c r="U163" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V163" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0"/>
+      <c r="B164" s="0"/>
+      <c r="C164" s="0"/>
+      <c r="D164" s="0"/>
+      <c r="E164" s="0"/>
+      <c r="F164" s="0"/>
+      <c r="G164" s="0"/>
+      <c r="H164" s="0"/>
+      <c r="I164" s="0"/>
+      <c r="J164" s="0"/>
+      <c r="K164" s="0"/>
+      <c r="L164" s="0"/>
+      <c r="M164" s="0"/>
+      <c r="N164" s="0"/>
+      <c r="O164" s="0"/>
+      <c r="P164" s="0"/>
+      <c r="Q164" s="0"/>
+      <c r="R164" s="0"/>
+      <c r="S164" s="0"/>
+      <c r="T164" s="0"/>
+      <c r="U164" s="0"/>
+      <c r="V164" s="0"/>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0"/>
+      <c r="B165" s="0"/>
+      <c r="C165" s="0"/>
+      <c r="D165" s="0"/>
+      <c r="E165" s="0"/>
+      <c r="F165" s="0"/>
+      <c r="G165" s="0"/>
+      <c r="H165" s="0"/>
+      <c r="I165" s="0"/>
+      <c r="J165" s="0"/>
+      <c r="K165" s="0"/>
+      <c r="L165" s="0"/>
+      <c r="M165" s="0"/>
+      <c r="N165" s="0"/>
+      <c r="O165" s="0"/>
+      <c r="P165" s="0"/>
+      <c r="Q165" s="0"/>
+      <c r="R165" s="0"/>
+      <c r="S165" s="0"/>
+      <c r="T165" s="0"/>
+      <c r="U165" s="0"/>
+      <c r="V165" s="0"/>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0"/>
+      <c r="B166" s="0"/>
+      <c r="C166" s="0"/>
+      <c r="D166" s="0"/>
+      <c r="E166" s="0"/>
+      <c r="F166" s="0"/>
+      <c r="G166" s="0"/>
+      <c r="H166" s="0"/>
+      <c r="I166" s="0"/>
+      <c r="J166" s="0"/>
+      <c r="K166" s="0"/>
+      <c r="L166" s="0"/>
+      <c r="M166" s="0"/>
+      <c r="N166" s="0"/>
+      <c r="O166" s="0"/>
+      <c r="P166" s="0"/>
+      <c r="Q166" s="0"/>
+      <c r="R166" s="0"/>
+      <c r="S166" s="0"/>
+      <c r="T166" s="0"/>
+      <c r="U166" s="0"/>
+      <c r="V166" s="0"/>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0"/>
+      <c r="B167" s="0"/>
+      <c r="C167" s="0"/>
+      <c r="D167" s="0"/>
+      <c r="E167" s="0"/>
+      <c r="F167" s="0"/>
+      <c r="G167" s="0"/>
+      <c r="H167" s="0"/>
+      <c r="I167" s="0"/>
+      <c r="J167" s="0"/>
+      <c r="K167" s="0"/>
+      <c r="L167" s="0"/>
+      <c r="M167" s="0"/>
+      <c r="N167" s="0"/>
+      <c r="O167" s="0"/>
+      <c r="P167" s="0"/>
+      <c r="Q167" s="0"/>
+      <c r="R167" s="0"/>
+      <c r="S167" s="0"/>
+      <c r="T167" s="0"/>
+      <c r="U167" s="0"/>
+      <c r="V167" s="0"/>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0"/>
+      <c r="B168" s="0"/>
+      <c r="C168" s="0"/>
+      <c r="D168" s="0"/>
+      <c r="E168" s="0"/>
+      <c r="F168" s="0"/>
+      <c r="G168" s="0"/>
+      <c r="H168" s="0"/>
+      <c r="I168" s="0"/>
+      <c r="J168" s="0"/>
+      <c r="K168" s="0"/>
+      <c r="L168" s="0"/>
+      <c r="M168" s="0"/>
+      <c r="N168" s="0"/>
+      <c r="O168" s="0"/>
+      <c r="P168" s="0"/>
+      <c r="Q168" s="0"/>
+      <c r="R168" s="0"/>
+      <c r="S168" s="0"/>
+      <c r="T168" s="0"/>
+      <c r="U168" s="0"/>
+      <c r="V168" s="0"/>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0"/>
+      <c r="B169" s="0"/>
+      <c r="C169" s="0"/>
+      <c r="D169" s="0"/>
+      <c r="E169" s="0"/>
+      <c r="F169" s="0"/>
+      <c r="G169" s="0"/>
+      <c r="H169" s="0"/>
+      <c r="I169" s="0"/>
+      <c r="J169" s="0"/>
+      <c r="K169" s="0"/>
+      <c r="L169" s="0"/>
+      <c r="M169" s="0"/>
+      <c r="N169" s="0"/>
+      <c r="O169" s="0"/>
+      <c r="P169" s="0"/>
+      <c r="Q169" s="0"/>
+      <c r="R169" s="0"/>
+      <c r="S169" s="0"/>
+      <c r="T169" s="0"/>
+      <c r="U169" s="0"/>
+      <c r="V169" s="0"/>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0"/>
+      <c r="B170" s="0"/>
+      <c r="C170" s="0"/>
+      <c r="D170" s="0"/>
+      <c r="E170" s="0"/>
+      <c r="F170" s="0"/>
+      <c r="G170" s="0"/>
+      <c r="H170" s="0"/>
+      <c r="I170" s="0"/>
+      <c r="J170" s="0"/>
+      <c r="K170" s="0"/>
+      <c r="L170" s="0"/>
+      <c r="M170" s="0"/>
+      <c r="N170" s="0"/>
+      <c r="O170" s="0"/>
+      <c r="P170" s="0"/>
+      <c r="Q170" s="0"/>
+      <c r="R170" s="0"/>
+      <c r="S170" s="0"/>
+      <c r="T170" s="0"/>
+      <c r="U170" s="0"/>
+      <c r="V170" s="0"/>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0"/>
+      <c r="B171" s="0"/>
+      <c r="C171" s="0"/>
+      <c r="D171" s="0"/>
+      <c r="E171" s="0"/>
+      <c r="F171" s="0"/>
+      <c r="G171" s="0"/>
+      <c r="H171" s="0"/>
+      <c r="I171" s="0"/>
+      <c r="J171" s="0"/>
+      <c r="K171" s="0"/>
+      <c r="L171" s="0"/>
+      <c r="M171" s="0"/>
+      <c r="N171" s="0"/>
+      <c r="O171" s="0"/>
+      <c r="P171" s="0"/>
+      <c r="Q171" s="0"/>
+      <c r="R171" s="0"/>
+      <c r="S171" s="0"/>
+      <c r="T171" s="0"/>
+      <c r="U171" s="0"/>
+      <c r="V171" s="0"/>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0"/>
+      <c r="B172" s="0"/>
+      <c r="C172" s="0"/>
+      <c r="D172" s="0"/>
+      <c r="E172" s="0"/>
+      <c r="F172" s="0"/>
+      <c r="G172" s="0"/>
+      <c r="H172" s="0"/>
+      <c r="I172" s="0"/>
+      <c r="J172" s="0"/>
+      <c r="K172" s="0"/>
+      <c r="L172" s="0"/>
+      <c r="M172" s="0"/>
+      <c r="N172" s="0"/>
+      <c r="O172" s="0"/>
+      <c r="P172" s="0"/>
+      <c r="Q172" s="0"/>
+      <c r="R172" s="0"/>
+      <c r="S172" s="0"/>
+      <c r="T172" s="0"/>
+      <c r="U172" s="0"/>
+      <c r="V172" s="0"/>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0"/>
+      <c r="B173" s="0"/>
+      <c r="C173" s="0"/>
+      <c r="D173" s="0"/>
+      <c r="E173" s="0"/>
+      <c r="F173" s="0"/>
+      <c r="G173" s="0"/>
+      <c r="H173" s="0"/>
+      <c r="I173" s="0"/>
+      <c r="J173" s="0"/>
+      <c r="K173" s="0"/>
+      <c r="L173" s="0"/>
+      <c r="M173" s="0"/>
+      <c r="N173" s="0"/>
+      <c r="O173" s="0"/>
+      <c r="P173" s="0"/>
+      <c r="Q173" s="0"/>
+      <c r="R173" s="0"/>
+      <c r="S173" s="0"/>
+      <c r="T173" s="0"/>
+      <c r="U173" s="0"/>
+      <c r="V173" s="0"/>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0"/>
+      <c r="B174" s="0"/>
+      <c r="C174" s="0"/>
+      <c r="D174" s="0"/>
+      <c r="E174" s="0"/>
+      <c r="F174" s="0"/>
+      <c r="G174" s="0"/>
+      <c r="H174" s="0"/>
+      <c r="I174" s="0"/>
+      <c r="J174" s="0"/>
+      <c r="K174" s="0"/>
+      <c r="L174" s="0"/>
+      <c r="M174" s="0"/>
+      <c r="N174" s="0"/>
+      <c r="O174" s="0"/>
+      <c r="P174" s="0"/>
+      <c r="Q174" s="0"/>
+      <c r="R174" s="0"/>
+      <c r="S174" s="0"/>
+      <c r="T174" s="0"/>
+      <c r="U174" s="0"/>
+      <c r="V174" s="0"/>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0"/>
+      <c r="B175" s="0"/>
+      <c r="C175" s="0"/>
+      <c r="D175" s="0"/>
+      <c r="E175" s="0"/>
+      <c r="F175" s="0"/>
+      <c r="G175" s="0"/>
+      <c r="H175" s="0"/>
+      <c r="I175" s="0"/>
+      <c r="J175" s="0"/>
+      <c r="K175" s="0"/>
+      <c r="L175" s="0"/>
+      <c r="M175" s="0"/>
+      <c r="N175" s="0"/>
+      <c r="O175" s="0"/>
+      <c r="P175" s="0"/>
+      <c r="Q175" s="0"/>
+      <c r="R175" s="0"/>
+      <c r="S175" s="0"/>
+      <c r="T175" s="0"/>
+      <c r="U175" s="0"/>
+      <c r="V175" s="0"/>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0"/>
+      <c r="B176" s="0"/>
+      <c r="C176" s="0"/>
+      <c r="D176" s="0"/>
+      <c r="E176" s="0"/>
+      <c r="F176" s="0"/>
+      <c r="G176" s="0"/>
+      <c r="H176" s="0"/>
+      <c r="I176" s="0"/>
+      <c r="J176" s="0"/>
+      <c r="K176" s="0"/>
+      <c r="L176" s="0"/>
+      <c r="M176" s="0"/>
+      <c r="N176" s="0"/>
+      <c r="O176" s="0"/>
+      <c r="P176" s="0"/>
+      <c r="Q176" s="0"/>
+      <c r="R176" s="0"/>
+      <c r="S176" s="0"/>
+      <c r="T176" s="0"/>
+      <c r="U176" s="0"/>
+      <c r="V176" s="0"/>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0"/>
+      <c r="B177" s="0"/>
+      <c r="C177" s="0"/>
+      <c r="D177" s="0"/>
+      <c r="E177" s="0"/>
+      <c r="F177" s="0"/>
+      <c r="G177" s="0"/>
+      <c r="H177" s="0"/>
+      <c r="I177" s="0"/>
+      <c r="J177" s="0"/>
+      <c r="K177" s="0"/>
+      <c r="L177" s="0"/>
+      <c r="M177" s="0"/>
+      <c r="N177" s="0"/>
+      <c r="O177" s="0"/>
+      <c r="P177" s="0"/>
+      <c r="Q177" s="0"/>
+      <c r="R177" s="0"/>
+      <c r="S177" s="0"/>
+      <c r="T177" s="0"/>
+      <c r="U177" s="0"/>
+      <c r="V177" s="0"/>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0"/>
+      <c r="B178" s="0"/>
+      <c r="C178" s="0"/>
+      <c r="D178" s="0"/>
+      <c r="E178" s="0"/>
+      <c r="F178" s="0"/>
+      <c r="G178" s="0"/>
+      <c r="H178" s="0"/>
+      <c r="I178" s="0"/>
+      <c r="J178" s="0"/>
+      <c r="K178" s="0"/>
+      <c r="L178" s="0"/>
+      <c r="M178" s="0"/>
+      <c r="N178" s="0"/>
+      <c r="O178" s="0"/>
+      <c r="P178" s="0"/>
+      <c r="Q178" s="0"/>
+      <c r="R178" s="0"/>
+      <c r="S178" s="0"/>
+      <c r="T178" s="0"/>
+      <c r="U178" s="0"/>
+      <c r="V178" s="0"/>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0"/>
+      <c r="B179" s="0"/>
+      <c r="C179" s="0"/>
+      <c r="D179" s="0"/>
+      <c r="E179" s="0"/>
+      <c r="F179" s="0"/>
+      <c r="G179" s="0"/>
+      <c r="H179" s="0"/>
+      <c r="I179" s="0"/>
+      <c r="J179" s="0"/>
+      <c r="K179" s="0"/>
+      <c r="L179" s="0"/>
+      <c r="M179" s="0"/>
+      <c r="N179" s="0"/>
+      <c r="O179" s="0"/>
+      <c r="P179" s="0"/>
+      <c r="Q179" s="0"/>
+      <c r="R179" s="0"/>
+      <c r="S179" s="0"/>
+      <c r="T179" s="0"/>
+      <c r="U179" s="0"/>
+      <c r="V179" s="0"/>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0"/>
+      <c r="B180" s="0"/>
+      <c r="C180" s="0"/>
+      <c r="D180" s="0"/>
+      <c r="E180" s="0"/>
+      <c r="F180" s="0"/>
+      <c r="G180" s="0"/>
+      <c r="H180" s="0"/>
+      <c r="I180" s="0"/>
+      <c r="J180" s="0"/>
+      <c r="K180" s="0"/>
+      <c r="L180" s="0"/>
+      <c r="M180" s="0"/>
+      <c r="N180" s="0"/>
+      <c r="O180" s="0"/>
+      <c r="P180" s="0"/>
+      <c r="Q180" s="0"/>
+      <c r="R180" s="0"/>
+      <c r="S180" s="0"/>
+      <c r="T180" s="0"/>
+      <c r="U180" s="0"/>
+      <c r="V180" s="0"/>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0"/>
+      <c r="B181" s="0"/>
+      <c r="C181" s="0"/>
+      <c r="D181" s="0"/>
+      <c r="E181" s="0"/>
+      <c r="F181" s="0"/>
+      <c r="G181" s="0"/>
+      <c r="H181" s="0"/>
+      <c r="I181" s="0"/>
+      <c r="J181" s="0"/>
+      <c r="K181" s="0"/>
+      <c r="L181" s="0"/>
+      <c r="M181" s="0"/>
+      <c r="N181" s="0"/>
+      <c r="O181" s="0"/>
+      <c r="P181" s="0"/>
+      <c r="Q181" s="0"/>
+      <c r="R181" s="0"/>
+      <c r="S181" s="0"/>
+      <c r="T181" s="0"/>
+      <c r="U181" s="0"/>
+      <c r="V181" s="0"/>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0"/>
+      <c r="B182" s="0"/>
+      <c r="C182" s="0"/>
+      <c r="D182" s="0"/>
+      <c r="E182" s="0"/>
+      <c r="F182" s="0"/>
+      <c r="G182" s="0"/>
+      <c r="H182" s="0"/>
+      <c r="I182" s="0"/>
+      <c r="J182" s="0"/>
+      <c r="K182" s="0"/>
+      <c r="L182" s="0"/>
+      <c r="M182" s="0"/>
+      <c r="N182" s="0"/>
+      <c r="O182" s="0"/>
+      <c r="P182" s="0"/>
+      <c r="Q182" s="0"/>
+      <c r="R182" s="0"/>
+      <c r="S182" s="0"/>
+      <c r="T182" s="0"/>
+      <c r="U182" s="0"/>
+      <c r="V182" s="0"/>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0"/>
+      <c r="B183" s="0"/>
+      <c r="C183" s="0"/>
+      <c r="D183" s="0"/>
+      <c r="E183" s="0"/>
+      <c r="F183" s="0"/>
+      <c r="G183" s="0"/>
+      <c r="H183" s="0"/>
+      <c r="I183" s="0"/>
+      <c r="J183" s="0"/>
+      <c r="K183" s="0"/>
+      <c r="L183" s="0"/>
+      <c r="M183" s="0"/>
+      <c r="N183" s="0"/>
+      <c r="O183" s="0"/>
+      <c r="P183" s="0"/>
+      <c r="Q183" s="0"/>
+      <c r="R183" s="0"/>
+      <c r="S183" s="0"/>
+      <c r="T183" s="0"/>
+      <c r="U183" s="0"/>
+      <c r="V183" s="0"/>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0"/>
+      <c r="B184" s="0"/>
+      <c r="C184" s="0"/>
+      <c r="D184" s="0"/>
+      <c r="E184" s="0"/>
+      <c r="F184" s="0"/>
+      <c r="G184" s="0"/>
+      <c r="H184" s="0"/>
+      <c r="I184" s="0"/>
+      <c r="J184" s="0"/>
+      <c r="K184" s="0"/>
+      <c r="L184" s="0"/>
+      <c r="M184" s="0"/>
+      <c r="N184" s="0"/>
+      <c r="O184" s="0"/>
+      <c r="P184" s="0"/>
+      <c r="Q184" s="0"/>
+      <c r="R184" s="0"/>
+      <c r="S184" s="0"/>
+      <c r="T184" s="0"/>
+      <c r="U184" s="0"/>
+      <c r="V184" s="0"/>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0"/>
+      <c r="B185" s="0"/>
+      <c r="C185" s="0"/>
+      <c r="D185" s="0"/>
+      <c r="E185" s="0"/>
+      <c r="F185" s="0"/>
+      <c r="G185" s="0"/>
+      <c r="H185" s="0"/>
+      <c r="I185" s="0"/>
+      <c r="J185" s="0"/>
+      <c r="K185" s="0"/>
+      <c r="L185" s="0"/>
+      <c r="M185" s="0"/>
+      <c r="N185" s="0"/>
+      <c r="O185" s="0"/>
+      <c r="P185" s="0"/>
+      <c r="Q185" s="0"/>
+      <c r="R185" s="0"/>
+      <c r="S185" s="0"/>
+      <c r="T185" s="0"/>
+      <c r="U185" s="0"/>
+      <c r="V185" s="0"/>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0"/>
+      <c r="B186" s="0"/>
+      <c r="C186" s="0"/>
+      <c r="D186" s="0"/>
+      <c r="E186" s="0"/>
+      <c r="F186" s="0"/>
+      <c r="G186" s="0"/>
+      <c r="H186" s="0"/>
+      <c r="I186" s="0"/>
+      <c r="J186" s="0"/>
+      <c r="K186" s="0"/>
+      <c r="L186" s="0"/>
+      <c r="M186" s="0"/>
+      <c r="N186" s="0"/>
+      <c r="O186" s="0"/>
+      <c r="P186" s="0"/>
+      <c r="Q186" s="0"/>
+      <c r="R186" s="0"/>
+      <c r="S186" s="0"/>
+      <c r="T186" s="0"/>
+      <c r="U186" s="0"/>
+      <c r="V186" s="0"/>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0"/>
+      <c r="B187" s="0"/>
+      <c r="C187" s="0"/>
+      <c r="D187" s="0"/>
+      <c r="E187" s="0"/>
+      <c r="F187" s="0"/>
+      <c r="G187" s="0"/>
+      <c r="H187" s="0"/>
+      <c r="I187" s="0"/>
+      <c r="J187" s="0"/>
+      <c r="K187" s="0"/>
+      <c r="L187" s="0"/>
+      <c r="M187" s="0"/>
+      <c r="N187" s="0"/>
+      <c r="O187" s="0"/>
+      <c r="P187" s="0"/>
+      <c r="Q187" s="0"/>
+      <c r="R187" s="0"/>
+      <c r="S187" s="0"/>
+      <c r="T187" s="0"/>
+      <c r="U187" s="0"/>
+      <c r="V187" s="0"/>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0"/>
+      <c r="B188" s="0"/>
+      <c r="C188" s="0"/>
+      <c r="D188" s="0"/>
+      <c r="E188" s="0"/>
+      <c r="F188" s="0"/>
+      <c r="G188" s="0"/>
+      <c r="H188" s="0"/>
+      <c r="I188" s="0"/>
+      <c r="J188" s="0"/>
+      <c r="K188" s="0"/>
+      <c r="L188" s="0"/>
+      <c r="M188" s="0"/>
+      <c r="N188" s="0"/>
+      <c r="O188" s="0"/>
+      <c r="P188" s="0"/>
+      <c r="Q188" s="0"/>
+      <c r="R188" s="0"/>
+      <c r="S188" s="0"/>
+      <c r="T188" s="0"/>
+      <c r="U188" s="0"/>
+      <c r="V188" s="0"/>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0"/>
+      <c r="B189" s="0"/>
+      <c r="C189" s="0"/>
+      <c r="D189" s="0"/>
+      <c r="E189" s="0"/>
+      <c r="F189" s="0"/>
+      <c r="G189" s="0"/>
+      <c r="H189" s="0"/>
+      <c r="I189" s="0"/>
+      <c r="J189" s="0"/>
+      <c r="K189" s="0"/>
+      <c r="L189" s="0"/>
+      <c r="M189" s="0"/>
+      <c r="N189" s="0"/>
+      <c r="O189" s="0"/>
+      <c r="P189" s="0"/>
+      <c r="Q189" s="0"/>
+      <c r="R189" s="0"/>
+      <c r="S189" s="0"/>
+      <c r="T189" s="0"/>
+      <c r="U189" s="0"/>
+      <c r="V189" s="0"/>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0"/>
+      <c r="B190" s="0"/>
+      <c r="C190" s="0"/>
+      <c r="D190" s="0"/>
+      <c r="E190" s="0"/>
+      <c r="F190" s="0"/>
+      <c r="G190" s="0"/>
+      <c r="H190" s="0"/>
+      <c r="I190" s="0"/>
+      <c r="J190" s="0"/>
+      <c r="K190" s="0"/>
+      <c r="L190" s="0"/>
+      <c r="M190" s="0"/>
+      <c r="N190" s="0"/>
+      <c r="O190" s="0"/>
+      <c r="P190" s="0"/>
+      <c r="Q190" s="0"/>
+      <c r="R190" s="0"/>
+      <c r="S190" s="0"/>
+      <c r="T190" s="0"/>
+      <c r="U190" s="0"/>
+      <c r="V190" s="0"/>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0"/>
+      <c r="B191" s="0"/>
+      <c r="C191" s="0"/>
+      <c r="D191" s="0"/>
+      <c r="E191" s="0"/>
+      <c r="F191" s="0"/>
+      <c r="G191" s="0"/>
+      <c r="H191" s="0"/>
+      <c r="I191" s="0"/>
+      <c r="J191" s="0"/>
+      <c r="K191" s="0"/>
+      <c r="L191" s="0"/>
+      <c r="M191" s="0"/>
+      <c r="N191" s="0"/>
+      <c r="O191" s="0"/>
+      <c r="P191" s="0"/>
+      <c r="Q191" s="0"/>
+      <c r="R191" s="0"/>
+      <c r="S191" s="0"/>
+      <c r="T191" s="0"/>
+      <c r="U191" s="0"/>
+      <c r="V191" s="0"/>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0"/>
+      <c r="B192" s="0"/>
+      <c r="C192" s="0"/>
+      <c r="D192" s="0"/>
+      <c r="E192" s="0"/>
+      <c r="F192" s="0"/>
+      <c r="G192" s="0"/>
+      <c r="H192" s="0"/>
+      <c r="I192" s="0"/>
+      <c r="J192" s="0"/>
+      <c r="K192" s="0"/>
+      <c r="L192" s="0"/>
+      <c r="M192" s="0"/>
+      <c r="N192" s="0"/>
+      <c r="O192" s="0"/>
+      <c r="P192" s="0"/>
+      <c r="Q192" s="0"/>
+      <c r="R192" s="0"/>
+      <c r="S192" s="0"/>
+      <c r="T192" s="0"/>
+      <c r="U192" s="0"/>
+      <c r="V192" s="0"/>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0"/>
+      <c r="B193" s="0"/>
+      <c r="C193" s="0"/>
+      <c r="D193" s="0"/>
+      <c r="E193" s="0"/>
+      <c r="F193" s="0"/>
+      <c r="G193" s="0"/>
+      <c r="H193" s="0"/>
+      <c r="I193" s="0"/>
+      <c r="J193" s="0"/>
+      <c r="K193" s="0"/>
+      <c r="L193" s="0"/>
+      <c r="M193" s="0"/>
+      <c r="N193" s="0"/>
+      <c r="O193" s="0"/>
+      <c r="P193" s="0"/>
+      <c r="Q193" s="0"/>
+      <c r="R193" s="0"/>
+      <c r="S193" s="0"/>
+      <c r="T193" s="0"/>
+      <c r="U193" s="0"/>
+      <c r="V193" s="0"/>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0"/>
+      <c r="B194" s="0"/>
+      <c r="C194" s="0"/>
+      <c r="D194" s="0"/>
+      <c r="E194" s="0"/>
+      <c r="F194" s="0"/>
+      <c r="G194" s="0"/>
+      <c r="H194" s="0"/>
+      <c r="I194" s="0"/>
+      <c r="J194" s="0"/>
+      <c r="K194" s="0"/>
+      <c r="L194" s="0"/>
+      <c r="M194" s="0"/>
+      <c r="N194" s="0"/>
+      <c r="O194" s="0"/>
+      <c r="P194" s="0"/>
+      <c r="Q194" s="0"/>
+      <c r="R194" s="0"/>
+      <c r="S194" s="0"/>
+      <c r="T194" s="0"/>
+      <c r="U194" s="0"/>
+      <c r="V194" s="0"/>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0"/>
+      <c r="B195" s="0"/>
+      <c r="C195" s="0"/>
+      <c r="D195" s="0"/>
+      <c r="E195" s="0"/>
+      <c r="F195" s="0"/>
+      <c r="G195" s="0"/>
+      <c r="H195" s="0"/>
+      <c r="I195" s="0"/>
+      <c r="J195" s="0"/>
+      <c r="K195" s="0"/>
+      <c r="L195" s="0"/>
+      <c r="M195" s="0"/>
+      <c r="N195" s="0"/>
+      <c r="O195" s="0"/>
+      <c r="P195" s="0"/>
+      <c r="Q195" s="0"/>
+      <c r="R195" s="0"/>
+      <c r="S195" s="0"/>
+      <c r="T195" s="0"/>
+      <c r="U195" s="0"/>
+      <c r="V195" s="0"/>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0"/>
+      <c r="B196" s="0"/>
+      <c r="C196" s="0"/>
+      <c r="D196" s="0"/>
+      <c r="E196" s="0"/>
+      <c r="F196" s="0"/>
+      <c r="G196" s="0"/>
+      <c r="H196" s="0"/>
+      <c r="I196" s="0"/>
+      <c r="J196" s="0"/>
+      <c r="K196" s="0"/>
+      <c r="L196" s="0"/>
+      <c r="M196" s="0"/>
+      <c r="N196" s="0"/>
+      <c r="O196" s="0"/>
+      <c r="P196" s="0"/>
+      <c r="Q196" s="0"/>
+      <c r="R196" s="0"/>
+      <c r="S196" s="0"/>
+      <c r="T196" s="0"/>
+      <c r="U196" s="0"/>
+      <c r="V196" s="0"/>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0"/>
+      <c r="B197" s="0"/>
+      <c r="C197" s="0"/>
+      <c r="D197" s="0"/>
+      <c r="E197" s="0"/>
+      <c r="F197" s="0"/>
+      <c r="G197" s="0"/>
+      <c r="H197" s="0"/>
+      <c r="I197" s="0"/>
+      <c r="J197" s="0"/>
+      <c r="K197" s="0"/>
+      <c r="L197" s="0"/>
+      <c r="M197" s="0"/>
+      <c r="N197" s="0"/>
+      <c r="O197" s="0"/>
+      <c r="P197" s="0"/>
+      <c r="Q197" s="0"/>
+      <c r="R197" s="0"/>
+      <c r="S197" s="0"/>
+      <c r="T197" s="0"/>
+      <c r="U197" s="0"/>
+      <c r="V197" s="0"/>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0"/>
+      <c r="B198" s="0"/>
+      <c r="C198" s="0"/>
+      <c r="D198" s="0"/>
+      <c r="E198" s="0"/>
+      <c r="F198" s="0"/>
+      <c r="G198" s="0"/>
+      <c r="H198" s="0"/>
+      <c r="I198" s="0"/>
+      <c r="J198" s="0"/>
+      <c r="K198" s="0"/>
+      <c r="L198" s="0"/>
+      <c r="M198" s="0"/>
+      <c r="N198" s="0"/>
+      <c r="O198" s="0"/>
+      <c r="P198" s="0"/>
+      <c r="Q198" s="0"/>
+      <c r="R198" s="0"/>
+      <c r="S198" s="0"/>
+      <c r="T198" s="0"/>
+      <c r="U198" s="0"/>
+      <c r="V198" s="0"/>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0"/>
+      <c r="B199" s="0"/>
+      <c r="C199" s="0"/>
+      <c r="D199" s="0"/>
+      <c r="E199" s="0"/>
+      <c r="F199" s="0"/>
+      <c r="G199" s="0"/>
+      <c r="H199" s="0"/>
+      <c r="I199" s="0"/>
+      <c r="J199" s="0"/>
+      <c r="K199" s="0"/>
+      <c r="L199" s="0"/>
+      <c r="M199" s="0"/>
+      <c r="N199" s="0"/>
+      <c r="O199" s="0"/>
+      <c r="P199" s="0"/>
+      <c r="Q199" s="0"/>
+      <c r="R199" s="0"/>
+      <c r="S199" s="0"/>
+      <c r="T199" s="0"/>
+      <c r="U199" s="0"/>
+      <c r="V199" s="0"/>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0"/>
+      <c r="B200" s="0"/>
+      <c r="C200" s="0"/>
+      <c r="D200" s="0"/>
+      <c r="E200" s="0"/>
+      <c r="F200" s="0"/>
+      <c r="G200" s="0"/>
+      <c r="H200" s="0"/>
+      <c r="I200" s="0"/>
+      <c r="J200" s="0"/>
+      <c r="K200" s="0"/>
+      <c r="L200" s="0"/>
+      <c r="M200" s="0"/>
+      <c r="N200" s="0"/>
+      <c r="O200" s="0"/>
+      <c r="P200" s="0"/>
+      <c r="Q200" s="0"/>
+      <c r="R200" s="0"/>
+      <c r="S200" s="0"/>
+      <c r="T200" s="0"/>
+      <c r="U200" s="0"/>
+      <c r="V200" s="0"/>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0"/>
+      <c r="B201" s="0"/>
+      <c r="C201" s="0"/>
+      <c r="D201" s="0"/>
+      <c r="E201" s="0"/>
+      <c r="F201" s="0"/>
+      <c r="G201" s="0"/>
+      <c r="H201" s="0"/>
+      <c r="I201" s="0"/>
+      <c r="J201" s="0"/>
+      <c r="K201" s="0"/>
+      <c r="L201" s="0"/>
+      <c r="M201" s="0"/>
+      <c r="N201" s="0"/>
+      <c r="O201" s="0"/>
+      <c r="P201" s="0"/>
+      <c r="Q201" s="0"/>
+      <c r="R201" s="0"/>
+      <c r="S201" s="0"/>
+      <c r="T201" s="0"/>
+      <c r="U201" s="0"/>
+      <c r="V201" s="0"/>
+    </row>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0"/>
+      <c r="B202" s="0"/>
+      <c r="C202" s="0"/>
+      <c r="D202" s="0"/>
+      <c r="E202" s="0"/>
+      <c r="F202" s="0"/>
+      <c r="G202" s="0"/>
+      <c r="H202" s="0"/>
+      <c r="I202" s="0"/>
+      <c r="J202" s="0"/>
+      <c r="K202" s="0"/>
+      <c r="L202" s="0"/>
+      <c r="M202" s="0"/>
+      <c r="N202" s="0"/>
+      <c r="O202" s="0"/>
+      <c r="P202" s="0"/>
+      <c r="Q202" s="0"/>
+      <c r="R202" s="0"/>
+      <c r="S202" s="0"/>
+      <c r="T202" s="0"/>
+      <c r="U202" s="0"/>
+      <c r="V202" s="0"/>
+    </row>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0"/>
+      <c r="B203" s="0"/>
+      <c r="C203" s="0"/>
+      <c r="D203" s="0"/>
+      <c r="E203" s="0"/>
+      <c r="F203" s="0"/>
+      <c r="G203" s="0"/>
+      <c r="H203" s="0"/>
+      <c r="I203" s="0"/>
+      <c r="J203" s="0"/>
+      <c r="K203" s="0"/>
+      <c r="L203" s="0"/>
+      <c r="M203" s="0"/>
+      <c r="N203" s="0"/>
+      <c r="O203" s="0"/>
+      <c r="P203" s="0"/>
+      <c r="Q203" s="0"/>
+      <c r="R203" s="0"/>
+      <c r="S203" s="0"/>
+      <c r="T203" s="0"/>
+      <c r="U203" s="0"/>
+      <c r="V203" s="0"/>
+    </row>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0"/>
+      <c r="B204" s="0"/>
+      <c r="C204" s="0"/>
+      <c r="D204" s="0"/>
+      <c r="E204" s="0"/>
+      <c r="F204" s="0"/>
+      <c r="G204" s="0"/>
+      <c r="H204" s="0"/>
+      <c r="I204" s="0"/>
+      <c r="J204" s="0"/>
+      <c r="K204" s="0"/>
+      <c r="L204" s="0"/>
+      <c r="M204" s="0"/>
+      <c r="N204" s="0"/>
+      <c r="O204" s="0"/>
+      <c r="P204" s="0"/>
+      <c r="Q204" s="0"/>
+      <c r="R204" s="0"/>
+      <c r="S204" s="0"/>
+      <c r="T204" s="0"/>
+      <c r="U204" s="0"/>
+      <c r="V204" s="0"/>
+    </row>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0"/>
+      <c r="B205" s="0"/>
+      <c r="C205" s="0"/>
+      <c r="D205" s="0"/>
+      <c r="E205" s="0"/>
+      <c r="F205" s="0"/>
+      <c r="G205" s="0"/>
+      <c r="H205" s="0"/>
+      <c r="I205" s="0"/>
+      <c r="J205" s="0"/>
+      <c r="K205" s="0"/>
+      <c r="L205" s="0"/>
+      <c r="M205" s="0"/>
+      <c r="N205" s="0"/>
+      <c r="O205" s="0"/>
+      <c r="P205" s="0"/>
+      <c r="Q205" s="0"/>
+      <c r="R205" s="0"/>
+      <c r="S205" s="0"/>
+      <c r="T205" s="0"/>
+      <c r="U205" s="0"/>
+      <c r="V205" s="0"/>
+    </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0"/>
+      <c r="B206" s="0"/>
+      <c r="C206" s="0"/>
+      <c r="D206" s="0"/>
+      <c r="E206" s="0"/>
+      <c r="F206" s="0"/>
+      <c r="G206" s="0"/>
+      <c r="H206" s="0"/>
+      <c r="I206" s="0"/>
+      <c r="J206" s="0"/>
+      <c r="K206" s="0"/>
+      <c r="L206" s="0"/>
+      <c r="M206" s="0"/>
+      <c r="N206" s="0"/>
+      <c r="O206" s="0"/>
+      <c r="P206" s="0"/>
+      <c r="Q206" s="0"/>
+      <c r="R206" s="0"/>
+      <c r="S206" s="0"/>
+      <c r="T206" s="0"/>
+      <c r="U206" s="0"/>
+      <c r="V206" s="0"/>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0"/>
+      <c r="B207" s="0"/>
+      <c r="C207" s="0"/>
+      <c r="D207" s="0"/>
+      <c r="E207" s="0"/>
+      <c r="F207" s="0"/>
+      <c r="G207" s="0"/>
+      <c r="H207" s="0"/>
+      <c r="I207" s="0"/>
+      <c r="J207" s="0"/>
+      <c r="K207" s="0"/>
+      <c r="L207" s="0"/>
+      <c r="M207" s="0"/>
+      <c r="N207" s="0"/>
+      <c r="O207" s="0"/>
+      <c r="P207" s="0"/>
+      <c r="Q207" s="0"/>
+      <c r="R207" s="0"/>
+      <c r="S207" s="0"/>
+      <c r="T207" s="0"/>
+      <c r="U207" s="0"/>
+      <c r="V207" s="0"/>
+    </row>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0"/>
+      <c r="B208" s="0"/>
+      <c r="C208" s="0"/>
+      <c r="D208" s="0"/>
+      <c r="E208" s="0"/>
+      <c r="F208" s="0"/>
+      <c r="G208" s="0"/>
+      <c r="H208" s="0"/>
+      <c r="I208" s="0"/>
+      <c r="J208" s="0"/>
+      <c r="K208" s="0"/>
+      <c r="L208" s="0"/>
+      <c r="M208" s="0"/>
+      <c r="N208" s="0"/>
+      <c r="O208" s="0"/>
+      <c r="P208" s="0"/>
+      <c r="Q208" s="0"/>
+      <c r="R208" s="0"/>
+      <c r="S208" s="0"/>
+      <c r="T208" s="0"/>
+      <c r="U208" s="0"/>
+      <c r="V208" s="0"/>
+    </row>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0"/>
+      <c r="B209" s="0"/>
+      <c r="C209" s="0"/>
+      <c r="D209" s="0"/>
+      <c r="E209" s="0"/>
+      <c r="F209" s="0"/>
+      <c r="G209" s="0"/>
+      <c r="H209" s="0"/>
+      <c r="I209" s="0"/>
+      <c r="J209" s="0"/>
+      <c r="K209" s="0"/>
+      <c r="L209" s="0"/>
+      <c r="M209" s="0"/>
+      <c r="N209" s="0"/>
+      <c r="O209" s="0"/>
+      <c r="P209" s="0"/>
+      <c r="Q209" s="0"/>
+      <c r="R209" s="0"/>
+      <c r="S209" s="0"/>
+      <c r="T209" s="0"/>
+      <c r="U209" s="0"/>
+      <c r="V209" s="0"/>
+    </row>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0"/>
+      <c r="B210" s="0"/>
+      <c r="C210" s="0"/>
+      <c r="D210" s="0"/>
+      <c r="E210" s="0"/>
+      <c r="F210" s="0"/>
+      <c r="G210" s="0"/>
+      <c r="H210" s="0"/>
+      <c r="I210" s="0"/>
+      <c r="J210" s="0"/>
+      <c r="K210" s="0"/>
+      <c r="L210" s="0"/>
+      <c r="M210" s="0"/>
+      <c r="N210" s="0"/>
+      <c r="O210" s="0"/>
+      <c r="P210" s="0"/>
+      <c r="Q210" s="0"/>
+      <c r="R210" s="0"/>
+      <c r="S210" s="0"/>
+      <c r="T210" s="0"/>
+      <c r="U210" s="0"/>
+      <c r="V210" s="0"/>
+    </row>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0"/>
+      <c r="B211" s="0"/>
+      <c r="C211" s="0"/>
+      <c r="D211" s="0"/>
+      <c r="E211" s="0"/>
+      <c r="F211" s="0"/>
+      <c r="G211" s="0"/>
+      <c r="H211" s="0"/>
+      <c r="I211" s="0"/>
+      <c r="J211" s="0"/>
+      <c r="K211" s="0"/>
+      <c r="L211" s="0"/>
+      <c r="M211" s="0"/>
+      <c r="N211" s="0"/>
+      <c r="O211" s="0"/>
+      <c r="P211" s="0"/>
+      <c r="Q211" s="0"/>
+      <c r="R211" s="0"/>
+      <c r="S211" s="0"/>
+      <c r="T211" s="0"/>
+      <c r="U211" s="0"/>
+      <c r="V211" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
sync 04/08/23. bug fixes. add tests.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data_telepresence.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data_telepresence.xlsx
@@ -390,8 +390,8 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C363" activeCellId="0" sqref="C363"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P331" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z336" activeCellId="0" sqref="Z336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
bug fixes, and rework the characters in tele-presence.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data_telepresence.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data_telepresence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajit\PycharmProjects\sim_env_master\ethical_governor\blackboard\commonutils\cbr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajit\PycharmProjects\simulator_env\ethical_governor\blackboard\commonutils\cbr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5FA17D-94AA-4175-8C54-0C57887C8ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDC037-61FA-4D76-8926-019DA563E85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2125" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="44">
   <si>
     <t>case_id</t>
   </si>
@@ -300,9 +300,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -340,7 +340,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -446,7 +446,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -588,7 +588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -596,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W355"/>
+  <dimension ref="A1:W384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N211" sqref="N211"/>
+    <sheetView tabSelected="1" topLeftCell="M357" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U386" sqref="U386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20268,6 +20268,1511 @@
         <v>13</v>
       </c>
     </row>
+    <row r="356" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B356" t="s">
+        <v>21</v>
+      </c>
+      <c r="C356" t="b">
+        <v>0</v>
+      </c>
+      <c r="D356" t="s">
+        <v>41</v>
+      </c>
+      <c r="E356" t="s">
+        <v>23</v>
+      </c>
+      <c r="F356" t="b">
+        <v>0</v>
+      </c>
+      <c r="G356"/>
+      <c r="H356"/>
+      <c r="I356"/>
+      <c r="J356" t="b">
+        <v>0</v>
+      </c>
+      <c r="K356"/>
+      <c r="L356"/>
+      <c r="M356" t="b">
+        <v>0</v>
+      </c>
+      <c r="N356"/>
+      <c r="O356"/>
+      <c r="P356">
+        <v>1</v>
+      </c>
+      <c r="Q356"/>
+      <c r="R356"/>
+      <c r="S356"/>
+      <c r="T356"/>
+      <c r="U356" t="s">
+        <v>24</v>
+      </c>
+      <c r="V356" s="1">
+        <v>1</v>
+      </c>
+      <c r="W356" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="357" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B357" t="s">
+        <v>21</v>
+      </c>
+      <c r="C357" t="b">
+        <v>0</v>
+      </c>
+      <c r="D357" t="s">
+        <v>41</v>
+      </c>
+      <c r="E357" t="s">
+        <v>23</v>
+      </c>
+      <c r="F357" t="b">
+        <v>0</v>
+      </c>
+      <c r="G357"/>
+      <c r="H357"/>
+      <c r="I357"/>
+      <c r="J357" t="b">
+        <v>0</v>
+      </c>
+      <c r="K357"/>
+      <c r="L357"/>
+      <c r="M357" t="b">
+        <v>0</v>
+      </c>
+      <c r="N357"/>
+      <c r="O357"/>
+      <c r="P357">
+        <v>-0.7</v>
+      </c>
+      <c r="Q357"/>
+      <c r="R357"/>
+      <c r="S357"/>
+      <c r="T357"/>
+      <c r="U357" t="s">
+        <v>25</v>
+      </c>
+      <c r="V357" s="1">
+        <v>0</v>
+      </c>
+      <c r="W357" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="358" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B358" t="s">
+        <v>21</v>
+      </c>
+      <c r="C358" t="b">
+        <v>1</v>
+      </c>
+      <c r="D358" t="s">
+        <v>41</v>
+      </c>
+      <c r="E358"/>
+      <c r="F358" t="b">
+        <v>0</v>
+      </c>
+      <c r="G358"/>
+      <c r="H358"/>
+      <c r="I358"/>
+      <c r="J358" t="b">
+        <v>0</v>
+      </c>
+      <c r="K358"/>
+      <c r="L358"/>
+      <c r="M358" t="b">
+        <v>0</v>
+      </c>
+      <c r="N358"/>
+      <c r="O358"/>
+      <c r="P358">
+        <v>0</v>
+      </c>
+      <c r="Q358"/>
+      <c r="R358"/>
+      <c r="S358"/>
+      <c r="T358"/>
+      <c r="U358" t="s">
+        <v>26</v>
+      </c>
+      <c r="V358" s="1">
+        <v>1</v>
+      </c>
+      <c r="W358" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="359" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B359" t="s">
+        <v>21</v>
+      </c>
+      <c r="C359" t="b">
+        <v>1</v>
+      </c>
+      <c r="D359" t="s">
+        <v>41</v>
+      </c>
+      <c r="E359"/>
+      <c r="F359" t="b">
+        <v>0</v>
+      </c>
+      <c r="G359"/>
+      <c r="H359"/>
+      <c r="I359"/>
+      <c r="J359" t="b">
+        <v>0</v>
+      </c>
+      <c r="K359"/>
+      <c r="L359"/>
+      <c r="M359" t="b">
+        <v>0</v>
+      </c>
+      <c r="N359"/>
+      <c r="O359"/>
+      <c r="P359">
+        <v>-0.7</v>
+      </c>
+      <c r="Q359"/>
+      <c r="R359"/>
+      <c r="S359"/>
+      <c r="T359"/>
+      <c r="U359" t="s">
+        <v>25</v>
+      </c>
+      <c r="V359" s="1">
+        <v>0</v>
+      </c>
+      <c r="W359" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="360" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B360" t="s">
+        <v>21</v>
+      </c>
+      <c r="C360" t="b">
+        <v>1</v>
+      </c>
+      <c r="D360" t="s">
+        <v>41</v>
+      </c>
+      <c r="E360" t="s">
+        <v>27</v>
+      </c>
+      <c r="F360" t="b">
+        <v>0</v>
+      </c>
+      <c r="G360"/>
+      <c r="H360"/>
+      <c r="I360"/>
+      <c r="J360" t="b">
+        <v>0</v>
+      </c>
+      <c r="K360"/>
+      <c r="L360"/>
+      <c r="M360" t="b">
+        <v>0</v>
+      </c>
+      <c r="N360"/>
+      <c r="O360"/>
+      <c r="P360">
+        <v>1</v>
+      </c>
+      <c r="Q360"/>
+      <c r="R360"/>
+      <c r="S360"/>
+      <c r="T360"/>
+      <c r="U360" t="s">
+        <v>28</v>
+      </c>
+      <c r="V360" s="1">
+        <v>1</v>
+      </c>
+      <c r="W360" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="361" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B361" t="s">
+        <v>21</v>
+      </c>
+      <c r="C361" t="b">
+        <v>1</v>
+      </c>
+      <c r="D361" t="s">
+        <v>41</v>
+      </c>
+      <c r="E361" t="s">
+        <v>27</v>
+      </c>
+      <c r="F361" t="b">
+        <v>0</v>
+      </c>
+      <c r="G361"/>
+      <c r="H361"/>
+      <c r="I361"/>
+      <c r="J361" t="b">
+        <v>0</v>
+      </c>
+      <c r="K361"/>
+      <c r="L361"/>
+      <c r="M361" t="b">
+        <v>0</v>
+      </c>
+      <c r="N361"/>
+      <c r="O361"/>
+      <c r="P361">
+        <v>-0.7</v>
+      </c>
+      <c r="Q361"/>
+      <c r="R361"/>
+      <c r="S361"/>
+      <c r="T361"/>
+      <c r="U361" t="s">
+        <v>29</v>
+      </c>
+      <c r="V361" s="1">
+        <v>0</v>
+      </c>
+      <c r="W361" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="362" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B362" t="s">
+        <v>21</v>
+      </c>
+      <c r="C362" t="b">
+        <v>1</v>
+      </c>
+      <c r="D362" t="s">
+        <v>41</v>
+      </c>
+      <c r="E362"/>
+      <c r="F362" t="b">
+        <v>0</v>
+      </c>
+      <c r="G362"/>
+      <c r="H362"/>
+      <c r="I362"/>
+      <c r="J362" t="b">
+        <v>0</v>
+      </c>
+      <c r="K362"/>
+      <c r="L362"/>
+      <c r="M362" t="b">
+        <v>0</v>
+      </c>
+      <c r="N362"/>
+      <c r="O362"/>
+      <c r="P362">
+        <v>0</v>
+      </c>
+      <c r="Q362"/>
+      <c r="R362"/>
+      <c r="S362"/>
+      <c r="T362"/>
+      <c r="U362" t="s">
+        <v>26</v>
+      </c>
+      <c r="V362" s="1">
+        <v>1</v>
+      </c>
+      <c r="W362" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="363" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B363" t="s">
+        <v>21</v>
+      </c>
+      <c r="C363" t="b">
+        <v>1</v>
+      </c>
+      <c r="D363" t="s">
+        <v>41</v>
+      </c>
+      <c r="E363"/>
+      <c r="F363" t="b">
+        <v>0</v>
+      </c>
+      <c r="G363"/>
+      <c r="H363"/>
+      <c r="I363"/>
+      <c r="J363" t="b">
+        <v>0</v>
+      </c>
+      <c r="K363"/>
+      <c r="L363"/>
+      <c r="M363" t="b">
+        <v>0</v>
+      </c>
+      <c r="N363"/>
+      <c r="O363"/>
+      <c r="P363">
+        <v>-0.7</v>
+      </c>
+      <c r="Q363"/>
+      <c r="R363"/>
+      <c r="S363"/>
+      <c r="T363"/>
+      <c r="U363" t="s">
+        <v>25</v>
+      </c>
+      <c r="V363" s="1">
+        <v>0</v>
+      </c>
+      <c r="W363" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="364" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B364" t="s">
+        <v>21</v>
+      </c>
+      <c r="C364" t="b">
+        <v>1</v>
+      </c>
+      <c r="D364" t="s">
+        <v>41</v>
+      </c>
+      <c r="E364" t="s">
+        <v>27</v>
+      </c>
+      <c r="F364" t="b">
+        <v>0</v>
+      </c>
+      <c r="G364"/>
+      <c r="H364"/>
+      <c r="I364"/>
+      <c r="J364" t="b">
+        <v>0</v>
+      </c>
+      <c r="K364"/>
+      <c r="L364"/>
+      <c r="M364" t="b">
+        <v>0</v>
+      </c>
+      <c r="N364"/>
+      <c r="O364"/>
+      <c r="P364">
+        <v>1</v>
+      </c>
+      <c r="Q364"/>
+      <c r="R364"/>
+      <c r="S364"/>
+      <c r="T364"/>
+      <c r="U364" t="s">
+        <v>28</v>
+      </c>
+      <c r="V364" s="1">
+        <v>1</v>
+      </c>
+      <c r="W364" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="365" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B365" t="s">
+        <v>21</v>
+      </c>
+      <c r="C365" t="b">
+        <v>1</v>
+      </c>
+      <c r="D365" t="s">
+        <v>41</v>
+      </c>
+      <c r="E365" t="s">
+        <v>27</v>
+      </c>
+      <c r="F365" t="b">
+        <v>0</v>
+      </c>
+      <c r="G365"/>
+      <c r="H365"/>
+      <c r="I365"/>
+      <c r="J365" t="b">
+        <v>0</v>
+      </c>
+      <c r="K365"/>
+      <c r="L365"/>
+      <c r="M365" t="b">
+        <v>0</v>
+      </c>
+      <c r="N365"/>
+      <c r="O365"/>
+      <c r="P365">
+        <v>-0.7</v>
+      </c>
+      <c r="Q365"/>
+      <c r="R365"/>
+      <c r="S365"/>
+      <c r="T365"/>
+      <c r="U365" t="s">
+        <v>29</v>
+      </c>
+      <c r="V365" s="1">
+        <v>0</v>
+      </c>
+      <c r="W365" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="366" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B366" t="s">
+        <v>38</v>
+      </c>
+      <c r="C366" t="b">
+        <v>1</v>
+      </c>
+      <c r="D366" t="s">
+        <v>41</v>
+      </c>
+      <c r="E366"/>
+      <c r="F366" t="b">
+        <v>0</v>
+      </c>
+      <c r="G366"/>
+      <c r="H366"/>
+      <c r="I366"/>
+      <c r="J366" t="b">
+        <v>0</v>
+      </c>
+      <c r="K366"/>
+      <c r="L366"/>
+      <c r="M366" t="b">
+        <v>0</v>
+      </c>
+      <c r="N366"/>
+      <c r="O366"/>
+      <c r="P366">
+        <v>0</v>
+      </c>
+      <c r="Q366"/>
+      <c r="R366"/>
+      <c r="S366"/>
+      <c r="T366"/>
+      <c r="U366" t="s">
+        <v>26</v>
+      </c>
+      <c r="V366" s="1">
+        <v>1</v>
+      </c>
+      <c r="W366" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="367" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B367" t="s">
+        <v>38</v>
+      </c>
+      <c r="C367" t="b">
+        <v>1</v>
+      </c>
+      <c r="D367" t="s">
+        <v>41</v>
+      </c>
+      <c r="E367"/>
+      <c r="F367" t="b">
+        <v>0</v>
+      </c>
+      <c r="G367"/>
+      <c r="H367"/>
+      <c r="I367"/>
+      <c r="J367" t="b">
+        <v>0</v>
+      </c>
+      <c r="K367"/>
+      <c r="L367"/>
+      <c r="M367" t="b">
+        <v>0</v>
+      </c>
+      <c r="N367"/>
+      <c r="O367"/>
+      <c r="P367">
+        <v>-0.7</v>
+      </c>
+      <c r="Q367"/>
+      <c r="R367"/>
+      <c r="S367"/>
+      <c r="T367"/>
+      <c r="U367" t="s">
+        <v>25</v>
+      </c>
+      <c r="V367" s="1">
+        <v>0</v>
+      </c>
+      <c r="W367" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="368" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B368" t="s">
+        <v>38</v>
+      </c>
+      <c r="C368" t="b">
+        <v>1</v>
+      </c>
+      <c r="D368" t="s">
+        <v>41</v>
+      </c>
+      <c r="E368" t="s">
+        <v>27</v>
+      </c>
+      <c r="F368" t="b">
+        <v>0</v>
+      </c>
+      <c r="G368"/>
+      <c r="H368"/>
+      <c r="I368"/>
+      <c r="J368" t="b">
+        <v>0</v>
+      </c>
+      <c r="K368"/>
+      <c r="L368"/>
+      <c r="M368" t="b">
+        <v>0</v>
+      </c>
+      <c r="N368"/>
+      <c r="O368"/>
+      <c r="P368">
+        <v>1</v>
+      </c>
+      <c r="Q368"/>
+      <c r="R368"/>
+      <c r="S368"/>
+      <c r="T368"/>
+      <c r="U368" t="s">
+        <v>28</v>
+      </c>
+      <c r="V368" s="1">
+        <v>1</v>
+      </c>
+      <c r="W368" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="369" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B369" t="s">
+        <v>38</v>
+      </c>
+      <c r="C369" t="b">
+        <v>1</v>
+      </c>
+      <c r="D369" t="s">
+        <v>41</v>
+      </c>
+      <c r="E369" t="s">
+        <v>27</v>
+      </c>
+      <c r="F369" t="b">
+        <v>0</v>
+      </c>
+      <c r="G369"/>
+      <c r="H369"/>
+      <c r="I369"/>
+      <c r="J369" t="b">
+        <v>0</v>
+      </c>
+      <c r="K369"/>
+      <c r="L369"/>
+      <c r="M369" t="b">
+        <v>0</v>
+      </c>
+      <c r="N369"/>
+      <c r="O369"/>
+      <c r="P369">
+        <v>-0.7</v>
+      </c>
+      <c r="Q369"/>
+      <c r="R369"/>
+      <c r="S369"/>
+      <c r="T369"/>
+      <c r="U369" t="s">
+        <v>29</v>
+      </c>
+      <c r="V369" s="1">
+        <v>0</v>
+      </c>
+      <c r="W369" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="370" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B370" t="s">
+        <v>38</v>
+      </c>
+      <c r="C370" t="b">
+        <v>1</v>
+      </c>
+      <c r="D370" t="s">
+        <v>41</v>
+      </c>
+      <c r="E370"/>
+      <c r="F370" t="b">
+        <v>1</v>
+      </c>
+      <c r="G370" t="s">
+        <v>39</v>
+      </c>
+      <c r="H370" t="b">
+        <v>0</v>
+      </c>
+      <c r="I370" t="s">
+        <v>36</v>
+      </c>
+      <c r="J370" t="b">
+        <v>1</v>
+      </c>
+      <c r="K370" t="s">
+        <v>39</v>
+      </c>
+      <c r="L370" t="b">
+        <v>0</v>
+      </c>
+      <c r="M370" t="b">
+        <v>0</v>
+      </c>
+      <c r="N370"/>
+      <c r="O370"/>
+      <c r="P370">
+        <v>0</v>
+      </c>
+      <c r="Q370">
+        <v>1</v>
+      </c>
+      <c r="R370">
+        <v>-0.8</v>
+      </c>
+      <c r="S370">
+        <v>-0.2</v>
+      </c>
+      <c r="T370"/>
+      <c r="U370" t="s">
+        <v>26</v>
+      </c>
+      <c r="V370" s="1">
+        <v>0</v>
+      </c>
+      <c r="W370" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="371" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B371" t="s">
+        <v>38</v>
+      </c>
+      <c r="C371" t="b">
+        <v>1</v>
+      </c>
+      <c r="D371" t="s">
+        <v>41</v>
+      </c>
+      <c r="E371"/>
+      <c r="F371" t="b">
+        <v>1</v>
+      </c>
+      <c r="G371" t="s">
+        <v>39</v>
+      </c>
+      <c r="H371" t="b">
+        <v>0</v>
+      </c>
+      <c r="I371" t="s">
+        <v>36</v>
+      </c>
+      <c r="J371" t="b">
+        <v>1</v>
+      </c>
+      <c r="K371" t="s">
+        <v>39</v>
+      </c>
+      <c r="L371" t="b">
+        <v>0</v>
+      </c>
+      <c r="M371" t="b">
+        <v>0</v>
+      </c>
+      <c r="N371"/>
+      <c r="O371"/>
+      <c r="P371">
+        <v>-0.7</v>
+      </c>
+      <c r="Q371">
+        <v>-1</v>
+      </c>
+      <c r="R371">
+        <v>0.8</v>
+      </c>
+      <c r="S371">
+        <v>0.2</v>
+      </c>
+      <c r="T371"/>
+      <c r="U371" t="s">
+        <v>25</v>
+      </c>
+      <c r="V371" s="1">
+        <v>1</v>
+      </c>
+      <c r="W371" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="372" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B372" t="s">
+        <v>38</v>
+      </c>
+      <c r="C372" t="b">
+        <v>1</v>
+      </c>
+      <c r="D372" t="s">
+        <v>41</v>
+      </c>
+      <c r="E372" t="s">
+        <v>27</v>
+      </c>
+      <c r="F372" t="b">
+        <v>1</v>
+      </c>
+      <c r="G372" t="s">
+        <v>39</v>
+      </c>
+      <c r="H372" t="b">
+        <v>0</v>
+      </c>
+      <c r="I372" t="s">
+        <v>36</v>
+      </c>
+      <c r="J372" t="b">
+        <v>1</v>
+      </c>
+      <c r="K372" t="s">
+        <v>39</v>
+      </c>
+      <c r="L372" t="b">
+        <v>0</v>
+      </c>
+      <c r="M372" t="b">
+        <v>0</v>
+      </c>
+      <c r="N372"/>
+      <c r="O372"/>
+      <c r="P372">
+        <v>1</v>
+      </c>
+      <c r="Q372">
+        <v>1</v>
+      </c>
+      <c r="R372">
+        <v>-0.8</v>
+      </c>
+      <c r="S372">
+        <v>-0.2</v>
+      </c>
+      <c r="T372"/>
+      <c r="U372" t="s">
+        <v>28</v>
+      </c>
+      <c r="V372" s="1">
+        <v>0</v>
+      </c>
+      <c r="W372" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="373" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B373" t="s">
+        <v>38</v>
+      </c>
+      <c r="C373" t="b">
+        <v>1</v>
+      </c>
+      <c r="D373" t="s">
+        <v>41</v>
+      </c>
+      <c r="E373" t="s">
+        <v>27</v>
+      </c>
+      <c r="F373" t="b">
+        <v>1</v>
+      </c>
+      <c r="G373" t="s">
+        <v>39</v>
+      </c>
+      <c r="H373" t="b">
+        <v>0</v>
+      </c>
+      <c r="I373" t="s">
+        <v>36</v>
+      </c>
+      <c r="J373" t="b">
+        <v>1</v>
+      </c>
+      <c r="K373" t="s">
+        <v>39</v>
+      </c>
+      <c r="L373" t="b">
+        <v>0</v>
+      </c>
+      <c r="M373" t="b">
+        <v>0</v>
+      </c>
+      <c r="N373"/>
+      <c r="O373"/>
+      <c r="P373">
+        <v>-0.7</v>
+      </c>
+      <c r="Q373">
+        <v>-1</v>
+      </c>
+      <c r="R373">
+        <v>0.8</v>
+      </c>
+      <c r="S373">
+        <v>0.2</v>
+      </c>
+      <c r="T373"/>
+      <c r="U373" t="s">
+        <v>29</v>
+      </c>
+      <c r="V373" s="1">
+        <v>1</v>
+      </c>
+      <c r="W373" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="374" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B374" t="s">
+        <v>38</v>
+      </c>
+      <c r="C374" t="b">
+        <v>1</v>
+      </c>
+      <c r="D374" t="s">
+        <v>41</v>
+      </c>
+      <c r="E374"/>
+      <c r="F374" t="b">
+        <v>1</v>
+      </c>
+      <c r="G374" t="s">
+        <v>39</v>
+      </c>
+      <c r="H374" t="b">
+        <v>0</v>
+      </c>
+      <c r="I374" t="s">
+        <v>36</v>
+      </c>
+      <c r="J374" t="b">
+        <v>1</v>
+      </c>
+      <c r="K374" t="s">
+        <v>39</v>
+      </c>
+      <c r="L374" t="b">
+        <v>0</v>
+      </c>
+      <c r="M374" t="b">
+        <v>0</v>
+      </c>
+      <c r="N374"/>
+      <c r="O374"/>
+      <c r="P374">
+        <v>0</v>
+      </c>
+      <c r="Q374">
+        <v>1</v>
+      </c>
+      <c r="R374">
+        <v>-0.8</v>
+      </c>
+      <c r="S374">
+        <v>-0.2</v>
+      </c>
+      <c r="T374"/>
+      <c r="U374" t="s">
+        <v>26</v>
+      </c>
+      <c r="V374" s="1">
+        <v>0</v>
+      </c>
+      <c r="W374" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="375" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B375" t="s">
+        <v>38</v>
+      </c>
+      <c r="C375" t="b">
+        <v>1</v>
+      </c>
+      <c r="D375" t="s">
+        <v>41</v>
+      </c>
+      <c r="E375"/>
+      <c r="F375" t="b">
+        <v>1</v>
+      </c>
+      <c r="G375" t="s">
+        <v>39</v>
+      </c>
+      <c r="H375" t="b">
+        <v>0</v>
+      </c>
+      <c r="I375" t="s">
+        <v>36</v>
+      </c>
+      <c r="J375" t="b">
+        <v>1</v>
+      </c>
+      <c r="K375" t="s">
+        <v>39</v>
+      </c>
+      <c r="L375" t="b">
+        <v>0</v>
+      </c>
+      <c r="M375" t="b">
+        <v>0</v>
+      </c>
+      <c r="N375"/>
+      <c r="O375"/>
+      <c r="P375">
+        <v>-0.7</v>
+      </c>
+      <c r="Q375">
+        <v>-1</v>
+      </c>
+      <c r="R375">
+        <v>0.8</v>
+      </c>
+      <c r="S375">
+        <v>0.2</v>
+      </c>
+      <c r="T375"/>
+      <c r="U375" t="s">
+        <v>25</v>
+      </c>
+      <c r="V375" s="1">
+        <v>1</v>
+      </c>
+      <c r="W375" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="376" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B376" t="s">
+        <v>38</v>
+      </c>
+      <c r="C376" t="b">
+        <v>1</v>
+      </c>
+      <c r="D376" t="s">
+        <v>41</v>
+      </c>
+      <c r="E376" t="s">
+        <v>30</v>
+      </c>
+      <c r="F376" t="b">
+        <v>1</v>
+      </c>
+      <c r="G376" t="s">
+        <v>39</v>
+      </c>
+      <c r="H376" t="b">
+        <v>0</v>
+      </c>
+      <c r="I376" t="s">
+        <v>36</v>
+      </c>
+      <c r="J376" t="b">
+        <v>1</v>
+      </c>
+      <c r="K376" t="s">
+        <v>39</v>
+      </c>
+      <c r="L376" t="b">
+        <v>0</v>
+      </c>
+      <c r="M376" t="b">
+        <v>0</v>
+      </c>
+      <c r="N376"/>
+      <c r="O376"/>
+      <c r="P376">
+        <v>1</v>
+      </c>
+      <c r="Q376">
+        <v>1</v>
+      </c>
+      <c r="R376">
+        <v>-0.8</v>
+      </c>
+      <c r="S376">
+        <v>-0.2</v>
+      </c>
+      <c r="T376"/>
+      <c r="U376" t="s">
+        <v>31</v>
+      </c>
+      <c r="V376" s="1">
+        <v>0</v>
+      </c>
+      <c r="W376" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="377" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B377" t="s">
+        <v>38</v>
+      </c>
+      <c r="C377" t="b">
+        <v>1</v>
+      </c>
+      <c r="D377" t="s">
+        <v>41</v>
+      </c>
+      <c r="E377" t="s">
+        <v>30</v>
+      </c>
+      <c r="F377" t="b">
+        <v>1</v>
+      </c>
+      <c r="G377" t="s">
+        <v>39</v>
+      </c>
+      <c r="H377" t="b">
+        <v>0</v>
+      </c>
+      <c r="I377" t="s">
+        <v>36</v>
+      </c>
+      <c r="J377" t="b">
+        <v>1</v>
+      </c>
+      <c r="K377" t="s">
+        <v>39</v>
+      </c>
+      <c r="L377" t="b">
+        <v>0</v>
+      </c>
+      <c r="M377" t="b">
+        <v>0</v>
+      </c>
+      <c r="N377"/>
+      <c r="O377"/>
+      <c r="P377">
+        <v>-0.7</v>
+      </c>
+      <c r="Q377">
+        <v>-1</v>
+      </c>
+      <c r="R377">
+        <v>0.8</v>
+      </c>
+      <c r="S377">
+        <v>0.2</v>
+      </c>
+      <c r="T377"/>
+      <c r="U377" t="s">
+        <v>29</v>
+      </c>
+      <c r="V377" s="1">
+        <v>1</v>
+      </c>
+      <c r="W377" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="378" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B378" t="s">
+        <v>38</v>
+      </c>
+      <c r="C378" t="b">
+        <v>1</v>
+      </c>
+      <c r="D378" t="s">
+        <v>41</v>
+      </c>
+      <c r="E378"/>
+      <c r="F378" t="b">
+        <v>1</v>
+      </c>
+      <c r="G378" t="s">
+        <v>39</v>
+      </c>
+      <c r="H378" t="b">
+        <v>0</v>
+      </c>
+      <c r="I378" t="s">
+        <v>36</v>
+      </c>
+      <c r="J378" t="b">
+        <v>1</v>
+      </c>
+      <c r="K378" t="s">
+        <v>39</v>
+      </c>
+      <c r="L378" t="b">
+        <v>0</v>
+      </c>
+      <c r="M378" t="b">
+        <v>0</v>
+      </c>
+      <c r="N378"/>
+      <c r="O378"/>
+      <c r="P378">
+        <v>0</v>
+      </c>
+      <c r="Q378">
+        <v>1</v>
+      </c>
+      <c r="R378">
+        <v>-0.8</v>
+      </c>
+      <c r="S378">
+        <v>-0.2</v>
+      </c>
+      <c r="T378"/>
+      <c r="U378" t="s">
+        <v>26</v>
+      </c>
+      <c r="V378" s="1">
+        <v>0</v>
+      </c>
+      <c r="W378" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="379" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B379" t="s">
+        <v>38</v>
+      </c>
+      <c r="C379" t="b">
+        <v>1</v>
+      </c>
+      <c r="D379" t="s">
+        <v>41</v>
+      </c>
+      <c r="E379"/>
+      <c r="F379" t="b">
+        <v>1</v>
+      </c>
+      <c r="G379" t="s">
+        <v>39</v>
+      </c>
+      <c r="H379" t="b">
+        <v>0</v>
+      </c>
+      <c r="I379" t="s">
+        <v>36</v>
+      </c>
+      <c r="J379" t="b">
+        <v>1</v>
+      </c>
+      <c r="K379" t="s">
+        <v>39</v>
+      </c>
+      <c r="L379" t="b">
+        <v>0</v>
+      </c>
+      <c r="M379" t="b">
+        <v>0</v>
+      </c>
+      <c r="N379"/>
+      <c r="O379"/>
+      <c r="P379">
+        <v>-0.7</v>
+      </c>
+      <c r="Q379">
+        <v>-1</v>
+      </c>
+      <c r="R379">
+        <v>0.8</v>
+      </c>
+      <c r="S379">
+        <v>0.2</v>
+      </c>
+      <c r="T379"/>
+      <c r="U379" t="s">
+        <v>25</v>
+      </c>
+      <c r="V379" s="1">
+        <v>1</v>
+      </c>
+      <c r="W379" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="380" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B380" t="s">
+        <v>38</v>
+      </c>
+      <c r="C380" t="b">
+        <v>1</v>
+      </c>
+      <c r="D380" t="s">
+        <v>41</v>
+      </c>
+      <c r="E380" t="s">
+        <v>30</v>
+      </c>
+      <c r="F380" t="b">
+        <v>1</v>
+      </c>
+      <c r="G380" t="s">
+        <v>39</v>
+      </c>
+      <c r="H380" t="b">
+        <v>0</v>
+      </c>
+      <c r="I380" t="s">
+        <v>36</v>
+      </c>
+      <c r="J380" t="b">
+        <v>1</v>
+      </c>
+      <c r="K380" t="s">
+        <v>39</v>
+      </c>
+      <c r="L380" t="b">
+        <v>0</v>
+      </c>
+      <c r="M380" t="b">
+        <v>0</v>
+      </c>
+      <c r="N380"/>
+      <c r="O380"/>
+      <c r="P380">
+        <v>1</v>
+      </c>
+      <c r="Q380">
+        <v>1</v>
+      </c>
+      <c r="R380">
+        <v>-0.8</v>
+      </c>
+      <c r="S380">
+        <v>-0.2</v>
+      </c>
+      <c r="T380"/>
+      <c r="U380" t="s">
+        <v>31</v>
+      </c>
+      <c r="V380" s="1">
+        <v>0</v>
+      </c>
+      <c r="W380" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="381" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B381" t="s">
+        <v>38</v>
+      </c>
+      <c r="C381" t="b">
+        <v>1</v>
+      </c>
+      <c r="D381" t="s">
+        <v>41</v>
+      </c>
+      <c r="E381" t="s">
+        <v>30</v>
+      </c>
+      <c r="F381" t="b">
+        <v>1</v>
+      </c>
+      <c r="G381" t="s">
+        <v>39</v>
+      </c>
+      <c r="H381" t="b">
+        <v>0</v>
+      </c>
+      <c r="I381" t="s">
+        <v>36</v>
+      </c>
+      <c r="J381" t="b">
+        <v>1</v>
+      </c>
+      <c r="K381" t="s">
+        <v>39</v>
+      </c>
+      <c r="L381" t="b">
+        <v>0</v>
+      </c>
+      <c r="M381" t="b">
+        <v>0</v>
+      </c>
+      <c r="N381"/>
+      <c r="O381"/>
+      <c r="P381">
+        <v>-0.7</v>
+      </c>
+      <c r="Q381">
+        <v>-1</v>
+      </c>
+      <c r="R381">
+        <v>0.8</v>
+      </c>
+      <c r="S381">
+        <v>0.2</v>
+      </c>
+      <c r="T381"/>
+      <c r="U381" t="s">
+        <v>29</v>
+      </c>
+      <c r="V381" s="1">
+        <v>1</v>
+      </c>
+      <c r="W381" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="382" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B382" t="s">
+        <v>38</v>
+      </c>
+      <c r="C382" t="b">
+        <v>1</v>
+      </c>
+      <c r="D382" t="s">
+        <v>41</v>
+      </c>
+      <c r="E382"/>
+      <c r="F382" t="b">
+        <v>1</v>
+      </c>
+      <c r="G382" t="s">
+        <v>39</v>
+      </c>
+      <c r="H382" t="b">
+        <v>0</v>
+      </c>
+      <c r="I382" t="s">
+        <v>36</v>
+      </c>
+      <c r="J382" t="b">
+        <v>1</v>
+      </c>
+      <c r="K382" t="s">
+        <v>39</v>
+      </c>
+      <c r="L382" t="b">
+        <v>0</v>
+      </c>
+      <c r="M382" t="b">
+        <v>0</v>
+      </c>
+      <c r="N382"/>
+      <c r="O382"/>
+      <c r="P382">
+        <v>0</v>
+      </c>
+      <c r="Q382">
+        <v>1</v>
+      </c>
+      <c r="R382">
+        <v>-0.8</v>
+      </c>
+      <c r="S382">
+        <v>-0.2</v>
+      </c>
+      <c r="T382"/>
+      <c r="U382" t="s">
+        <v>26</v>
+      </c>
+      <c r="V382" s="1">
+        <v>0</v>
+      </c>
+      <c r="W382" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="383" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B383" t="s">
+        <v>38</v>
+      </c>
+      <c r="C383" t="b">
+        <v>1</v>
+      </c>
+      <c r="D383" t="s">
+        <v>41</v>
+      </c>
+      <c r="E383"/>
+      <c r="F383" t="b">
+        <v>1</v>
+      </c>
+      <c r="G383" t="s">
+        <v>39</v>
+      </c>
+      <c r="H383" t="b">
+        <v>0</v>
+      </c>
+      <c r="I383" t="s">
+        <v>36</v>
+      </c>
+      <c r="J383" t="b">
+        <v>1</v>
+      </c>
+      <c r="K383" t="s">
+        <v>39</v>
+      </c>
+      <c r="L383" t="b">
+        <v>0</v>
+      </c>
+      <c r="M383" t="b">
+        <v>0</v>
+      </c>
+      <c r="N383"/>
+      <c r="O383"/>
+      <c r="P383">
+        <v>-0.7</v>
+      </c>
+      <c r="Q383">
+        <v>-1</v>
+      </c>
+      <c r="R383">
+        <v>0.8</v>
+      </c>
+      <c r="S383">
+        <v>0.2</v>
+      </c>
+      <c r="T383"/>
+      <c r="U383" t="s">
+        <v>25</v>
+      </c>
+      <c r="V383" s="1">
+        <v>1</v>
+      </c>
+      <c r="W383" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="384" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B384"/>
+      <c r="C384"/>
+      <c r="D384"/>
+      <c r="E384"/>
+      <c r="F384"/>
+      <c r="G384"/>
+      <c r="H384"/>
+      <c r="I384"/>
+      <c r="J384"/>
+      <c r="K384"/>
+      <c r="L384"/>
+      <c r="M384"/>
+      <c r="N384"/>
+      <c r="O384"/>
+      <c r="P384"/>
+      <c r="Q384"/>
+      <c r="R384"/>
+      <c r="S384"/>
+      <c r="T384"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
telepresence genralisability with the filelength bug.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data_telepresence.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data_telepresence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajit\PycharmProjects\simulator_env\ethical_governor\blackboard\commonutils\cbr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDC037-61FA-4D76-8926-019DA563E85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791171A8-9F63-4037-8A4F-1DD419FFFA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M357" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="U386" sqref="U386"/>
+    <sheetView tabSelected="1" topLeftCell="A366" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F386" sqref="F386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20269,6 +20269,9 @@
       </c>
     </row>
     <row r="356" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A356" s="17">
+        <v>355</v>
+      </c>
       <c r="B356" t="s">
         <v>21</v>
       </c>
@@ -20315,6 +20318,9 @@
       </c>
     </row>
     <row r="357" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A357" s="17">
+        <v>356</v>
+      </c>
       <c r="B357" t="s">
         <v>21</v>
       </c>
@@ -20361,6 +20367,9 @@
       </c>
     </row>
     <row r="358" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A358" s="17">
+        <v>357</v>
+      </c>
       <c r="B358" t="s">
         <v>21</v>
       </c>
@@ -20405,6 +20414,9 @@
       </c>
     </row>
     <row r="359" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A359" s="17">
+        <v>358</v>
+      </c>
       <c r="B359" t="s">
         <v>21</v>
       </c>
@@ -20449,6 +20461,9 @@
       </c>
     </row>
     <row r="360" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A360" s="17">
+        <v>359</v>
+      </c>
       <c r="B360" t="s">
         <v>21</v>
       </c>
@@ -20495,6 +20510,9 @@
       </c>
     </row>
     <row r="361" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A361" s="17">
+        <v>360</v>
+      </c>
       <c r="B361" t="s">
         <v>21</v>
       </c>
@@ -20541,6 +20559,9 @@
       </c>
     </row>
     <row r="362" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A362" s="17">
+        <v>361</v>
+      </c>
       <c r="B362" t="s">
         <v>21</v>
       </c>
@@ -20585,6 +20606,9 @@
       </c>
     </row>
     <row r="363" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A363" s="17">
+        <v>362</v>
+      </c>
       <c r="B363" t="s">
         <v>21</v>
       </c>
@@ -20629,6 +20653,9 @@
       </c>
     </row>
     <row r="364" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A364" s="17">
+        <v>363</v>
+      </c>
       <c r="B364" t="s">
         <v>21</v>
       </c>
@@ -20675,6 +20702,9 @@
       </c>
     </row>
     <row r="365" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A365" s="17">
+        <v>364</v>
+      </c>
       <c r="B365" t="s">
         <v>21</v>
       </c>
@@ -20721,6 +20751,9 @@
       </c>
     </row>
     <row r="366" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A366" s="17">
+        <v>365</v>
+      </c>
       <c r="B366" t="s">
         <v>38</v>
       </c>
@@ -20765,6 +20798,9 @@
       </c>
     </row>
     <row r="367" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A367" s="17">
+        <v>366</v>
+      </c>
       <c r="B367" t="s">
         <v>38</v>
       </c>
@@ -20809,6 +20845,9 @@
       </c>
     </row>
     <row r="368" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A368" s="17">
+        <v>367</v>
+      </c>
       <c r="B368" t="s">
         <v>38</v>
       </c>
@@ -20854,7 +20893,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="369" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A369" s="17">
+        <v>368</v>
+      </c>
       <c r="B369" t="s">
         <v>38</v>
       </c>
@@ -20900,7 +20942,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="370" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A370" s="17">
+        <v>369</v>
+      </c>
       <c r="B370" t="s">
         <v>38</v>
       </c>
@@ -20960,7 +21005,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="371" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A371" s="17">
+        <v>370</v>
+      </c>
       <c r="B371" t="s">
         <v>38</v>
       </c>
@@ -21020,7 +21068,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="372" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A372" s="17">
+        <v>371</v>
+      </c>
       <c r="B372" t="s">
         <v>38</v>
       </c>
@@ -21082,7 +21133,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="373" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A373" s="17">
+        <v>372</v>
+      </c>
       <c r="B373" t="s">
         <v>38</v>
       </c>
@@ -21144,7 +21198,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="374" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A374" s="17">
+        <v>373</v>
+      </c>
       <c r="B374" t="s">
         <v>38</v>
       </c>
@@ -21204,7 +21261,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="375" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A375" s="17">
+        <v>374</v>
+      </c>
       <c r="B375" t="s">
         <v>38</v>
       </c>
@@ -21264,7 +21324,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="376" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A376" s="17">
+        <v>375</v>
+      </c>
       <c r="B376" t="s">
         <v>38</v>
       </c>
@@ -21326,7 +21389,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="377" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A377" s="17">
+        <v>376</v>
+      </c>
       <c r="B377" t="s">
         <v>38</v>
       </c>
@@ -21388,7 +21454,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="378" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A378" s="17">
+        <v>377</v>
+      </c>
       <c r="B378" t="s">
         <v>38</v>
       </c>
@@ -21448,7 +21517,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="379" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A379" s="17">
+        <v>378</v>
+      </c>
       <c r="B379" t="s">
         <v>38</v>
       </c>
@@ -21508,7 +21580,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="380" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A380" s="17">
+        <v>379</v>
+      </c>
       <c r="B380" t="s">
         <v>38</v>
       </c>
@@ -21570,7 +21645,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="381" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A381" s="17">
+        <v>380</v>
+      </c>
       <c r="B381" t="s">
         <v>38</v>
       </c>
@@ -21632,7 +21710,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="382" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A382" s="17">
+        <v>381</v>
+      </c>
       <c r="B382" t="s">
         <v>38</v>
       </c>
@@ -21692,7 +21773,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="383" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A383" s="17">
+        <v>382</v>
+      </c>
       <c r="B383" t="s">
         <v>38</v>
       </c>
@@ -21752,7 +21836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="384" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B384"/>
       <c r="C384"/>
       <c r="D384"/>

</xml_diff>